<commit_message>
* Tinkered with parser.
</commit_message>
<xml_diff>
--- a/barlom-language/lexer/doc/TokenTypes.xlsx
+++ b/barlom-language/lexer/doc/TokenTypes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="354">
   <si>
     <t>Token Text</t>
   </si>
@@ -373,6 +373,12 @@
     <t>CONSTANT</t>
   </si>
   <si>
+    <t>context</t>
+  </si>
+  <si>
+    <t>CONTEXT</t>
+  </si>
+  <si>
     <t>data</t>
   </si>
   <si>
@@ -877,6 +883,12 @@
     <t>SYMBOL</t>
   </si>
   <si>
+    <t>#abc_def</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
     <t>TemplateLiteral</t>
   </si>
   <si>
@@ -983,12 +995,6 @@
   </si>
   <si>
     <t>USE</t>
-  </si>
-  <si>
-    <t>#abc</t>
-  </si>
-  <si>
-    <t>UserDefinedKeyWord</t>
   </si>
   <si>
     <t>UserDefinedLiteral_Braces</t>
@@ -1198,20 +1204,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E214"/>
+  <dimension ref="A1:E215"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A190" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E218" activeCellId="0" sqref="E218"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.1224489795918"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="75.5969387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="74.6479591836735"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2379,38 +2384,38 @@
       </c>
       <c r="E73" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B73,",    // ",C73," `",A73,"`    ",D73)</f>
+        <v>  CONTEXT,    // Keyword `context`    </v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="C74" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E74" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B74,",    // ",C74," `",A74,"`    ",D74)</f>
         <v>  DATA,    // Keyword `data`    </v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="str">
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="str">
         <f aca="false">"$2016-12-31T12:01:14.001-05:00$"</f>
         <v>$2016-12-31T12:01:14.001-05:00$</v>
       </c>
-      <c r="B74" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="C74" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E74" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B74,",    // ",C74," `",A74,"`    ",D74)</f>
-        <v>  DateTimeLiteral,    // Literal `$2016-12-31T12:01:14.001-05:00$`    </v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
-        <v>120</v>
-      </c>
       <c r="B75" s="0" t="s">
         <v>121</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E75" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B75,",    // ",C75," `",A75,"`    ",D75)</f>
-        <v>  DEFAULT,    // Keyword `default`    </v>
+        <v>  DateTimeLiteral,    // Literal `$2016-12-31T12:01:14.001-05:00$`    </v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2425,7 +2430,7 @@
       </c>
       <c r="E76" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B76,",    // ",C76," `",A76,"`    ",D76)</f>
-        <v>  DEFER,    // Keyword `defer`    </v>
+        <v>  DEFAULT,    // Keyword `default`    </v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2440,7 +2445,7 @@
       </c>
       <c r="E77" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B77,",    // ",C77," `",A77,"`    ",D77)</f>
-        <v>  DEFINE,    // Keyword `define`    </v>
+        <v>  DEFER,    // Keyword `defer`    </v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2455,7 +2460,7 @@
       </c>
       <c r="E78" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B78,",    // ",C78," `",A78,"`    ",D78)</f>
-        <v>  DELETE,    // Keyword `delete`    </v>
+        <v>  DEFINE,    // Keyword `define`    </v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2470,7 +2475,7 @@
       </c>
       <c r="E79" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B79,",    // ",C79," `",A79,"`    ",D79)</f>
-        <v>  DETECT,    // Keyword `detect`    </v>
+        <v>  DELETE,    // Keyword `delete`    </v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2485,111 +2490,111 @@
       </c>
       <c r="E80" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B80,",    // ",C80," `",A80,"`    ",D80)</f>
+        <v>  DETECT,    // Keyword `detect`    </v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="C81" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E81" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B81,",    // ",C81," `",A81,"`    ",D81)</f>
         <v>  DIV,    // Keyword `div`    </v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="str">
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="str">
         <f aca="false">"/="</f>
         <v>/=</v>
       </c>
-      <c r="B81" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="C81" s="0" t="s">
+      <c r="B82" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="C82" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="E81" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B81,",    // ",C81," `",A81,"`    ",D81)</f>
+      <c r="E82" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B82,",    // ",C82," `",A82,"`    ",D82)</f>
         <v>  DIVIDE_EQUALS,    // Operator `/=`    </v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="str">
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="str">
         <f aca="false">"/"</f>
         <v>/</v>
       </c>
-      <c r="B82" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="C82" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="E82" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B82,",    // ",C82," `",A82,"`    ",D82)</f>
-        <v>  DIVIDED_BY,    // Operator `/`    </v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="s">
-        <v>134</v>
-      </c>
       <c r="B83" s="0" t="s">
         <v>135</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="E83" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B83,",    // ",C83," `",A83,"`    ",D83)</f>
+        <v>  DIVIDED_BY,    // Operator `/`    </v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="B84" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="C84" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E84" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B84,",    // ",C84," `",A84,"`    ",D84)</f>
         <v>  DO,    // Keyword `do`    </v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="str">
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="str">
         <f aca="false">"/*...*/"</f>
         <v>/*...*/</v>
       </c>
-      <c r="B84" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="C84" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="D84" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="E84" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B84,",    // ",C84," `",A84,"`    ",D84)</f>
+      <c r="B85" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="C85" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="D85" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="E85" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B85,",    // ",C85," `",A85,"`    ",D85)</f>
         <v>  Documentation,    // Documentation `/*...*/`    Annotation documentation for an element</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="str">
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="str">
         <f aca="false">"."</f>
         <v>.</v>
       </c>
-      <c r="B85" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="C85" s="0" t="s">
+      <c r="B86" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="C86" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="E85" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B85,",    // ",C85," `",A85,"`    ",D85)</f>
+      <c r="E86" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B86,",    // ",C86," `",A86,"`    ",D86)</f>
         <v>  DOT,    // Punctuation `.`    </v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="0" t="str">
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="str">
         <f aca="false">"..."</f>
         <v>...</v>
       </c>
-      <c r="B86" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="C86" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="E86" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B86,",    // ",C86," `",A86,"`    ",D86)</f>
-        <v>  DOT_DOT_DOT,    // Punctuation `...`    </v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="0" t="s">
-        <v>140</v>
-      </c>
       <c r="B87" s="0" t="s">
         <v>141</v>
       </c>
@@ -2598,7 +2603,7 @@
       </c>
       <c r="E87" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B87,",    // ",C87," `",A87,"`    ",D87)</f>
-        <v>  DOT_QUESTION,    // Punctuation `.?`    </v>
+        <v>  DOT_DOT_DOT,    // Punctuation `...`    </v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2609,11 +2614,11 @@
         <v>143</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>7</v>
+        <v>109</v>
       </c>
       <c r="E88" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B88,",    // ",C88," `",A88,"`    ",D88)</f>
-        <v>  EDGE,    // Keyword `edge`    </v>
+        <v>  DOT_QUESTION,    // Punctuation `.?`    </v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2628,7 +2633,7 @@
       </c>
       <c r="E89" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B89,",    // ",C89," `",A89,"`    ",D89)</f>
-        <v>  ELSE,    // Keyword `else`    </v>
+        <v>  EDGE,    // Keyword `edge`    </v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2643,7 +2648,7 @@
       </c>
       <c r="E90" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B90,",    // ",C90," `",A90,"`    ",D90)</f>
-        <v>  END,    // Keyword `end`    </v>
+        <v>  ELSE,    // Keyword `else`    </v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2658,50 +2663,53 @@
       </c>
       <c r="E91" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B91,",    // ",C91," `",A91,"`    ",D91)</f>
+        <v>  END,    // Keyword `end`    </v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B92" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="C92" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E92" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B92,",    // ",C92," `",A92,"`    ",D92)</f>
         <v>  ENUMERATION,    // Keyword `enumeration`    </v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="0" t="str">
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="str">
         <f aca="false">"="</f>
         <v>=</v>
       </c>
-      <c r="B92" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="C92" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="E92" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B92,",    // ",C92," `",A92,"`    ",D92)</f>
-        <v>  EQUALS,    // Operator `=`    </v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="0" t="s">
-        <v>151</v>
-      </c>
       <c r="B93" s="0" t="s">
         <v>152</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="E93" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B93,",    // ",C93," `",A93,"`    ",D93)</f>
-        <v>  ERROR,    // Keyword `error`    </v>
+        <v>  EQUALS,    // Operator `=`    </v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="s">
+        <v>153</v>
+      </c>
       <c r="B94" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>154</v>
+        <v>7</v>
       </c>
       <c r="E94" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B94,",    // ",C94," `",A94,"`    ",D94)</f>
-        <v>  ErrorInvalidIdentifier,    // Error ``    </v>
+        <v>  ERROR,    // Keyword `error`    </v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2709,153 +2717,150 @@
         <v>155</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E95" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B95,",    // ",C95," `",A95,"`    ",D95)</f>
-        <v>  ErrorInvalidMultilineTextLiteral,    // Error ``    </v>
+        <v>  ErrorInvalidIdentifier,    // Error ``    </v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="C96" s="0" t="s">
         <v>156</v>
-      </c>
-      <c r="C96" s="0" t="s">
-        <v>154</v>
       </c>
       <c r="E96" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B96,",    // ",C96," `",A96,"`    ",D96)</f>
-        <v>  ErrorInvalidTextLiteral,    // Error ``    </v>
+        <v>  ErrorInvalidMultilineTextLiteral,    // Error ``    </v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E97" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B97,",    // ",C97," `",A97,"`    ",D97)</f>
-        <v>  ErrorInvalidTimeLiteral,    // Error ``    </v>
+        <v>  ErrorInvalidTextLiteral,    // Error ``    </v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E98" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B98,",    // ",C98," `",A98,"`    ",D98)</f>
-        <v>  ErrorUnclosedBlockComment,    // Error ``    </v>
+        <v>  ErrorInvalidTimeLiteral,    // Error ``    </v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E99" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B99,",    // ",C99," `",A99,"`    ",D99)</f>
-        <v>  ErrorUnclosedCodeLiteral,    // Error ``    </v>
+        <v>  ErrorUnclosedBlockComment,    // Error ``    </v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E100" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B100,",    // ",C100," `",A100,"`    ",D100)</f>
-        <v>  ErrorUnclosedLocationLiteral,    // Error ``    </v>
+        <v>  ErrorUnclosedCodeLiteral,    // Error ``    </v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E101" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B101,",    // ",C101," `",A101,"`    ",D101)</f>
-        <v>  ErrorUnclosedRegularExpression,    // Error ``    </v>
+        <v>  ErrorUnclosedLocationLiteral,    // Error ``    </v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E102" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B102,",    // ",C102," `",A102,"`    ",D102)</f>
-        <v>  ErrorUnclosedTemplate,    // Error ``    </v>
+        <v>  ErrorUnclosedRegularExpression,    // Error ``    </v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E103" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B103,",    // ",C103," `",A103,"`    ",D103)</f>
-        <v>  ErrorUnclosedTextLiteral,    // Error ``    </v>
+        <v>  ErrorUnclosedTemplate,    // Error ``    </v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E104" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B104,",    // ",C104," `",A104,"`    ",D104)</f>
-        <v>  ErrorUnclosedTextLiteralMultiline,    // Error ``    </v>
+        <v>  ErrorUnclosedTextLiteral,    // Error ``    </v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E105" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B105,",    // ",C105," `",A105,"`    ",D105)</f>
-        <v>  ErrorUnexpectedCharacter,    // Error ``    </v>
+        <v>  ErrorUnclosedTextLiteralMultiline,    // Error ``    </v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="0" t="s">
-        <v>166</v>
-      </c>
       <c r="B106" s="0" t="s">
         <v>167</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>7</v>
+        <v>156</v>
       </c>
       <c r="E106" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B106,",    // ",C106," `",A106,"`    ",D106)</f>
-        <v>  EXPECT,    // Keyword `expect`    </v>
+        <v>  ErrorUnexpectedCharacter,    // Error ``    </v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="2" t="s">
+      <c r="A107" s="0" t="s">
         <v>168</v>
       </c>
-      <c r="B107" s="2" t="s">
+      <c r="B107" s="0" t="s">
         <v>169</v>
       </c>
       <c r="C107" s="0" t="s">
@@ -2863,14 +2868,14 @@
       </c>
       <c r="E107" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B107,",    // ",C107," `",A107,"`    ",D107)</f>
-        <v>  FALSE,    // Keyword `false`    </v>
+        <v>  EXPECT,    // Keyword `expect`    </v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="0" t="s">
+      <c r="A108" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B108" s="0" t="s">
+      <c r="B108" s="2" t="s">
         <v>171</v>
       </c>
       <c r="C108" s="0" t="s">
@@ -2878,7 +2883,7 @@
       </c>
       <c r="E108" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B108,",    // ",C108," `",A108,"`    ",D108)</f>
-        <v>  FOR,    // Keyword `for`    </v>
+        <v>  FALSE,    // Keyword `false`    </v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2893,7 +2898,7 @@
       </c>
       <c r="E109" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B109,",    // ",C109," `",A109,"`    ",D109)</f>
-        <v>  FUNCTION,    // Keyword `function`    </v>
+        <v>  FOR,    // Keyword `for`    </v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2908,7 +2913,7 @@
       </c>
       <c r="E110" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B110,",    // ",C110," `",A110,"`    ",D110)</f>
-        <v>  GIVEN,    // Keyword `given`    </v>
+        <v>  FUNCTION,    // Keyword `function`    </v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2923,107 +2928,107 @@
       </c>
       <c r="E111" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B111,",    // ",C111," `",A111,"`    ",D111)</f>
+        <v>  GIVEN,    // Keyword `given`    </v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="B112" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="C112" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E112" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B112,",    // ",C112," `",A112,"`    ",D112)</f>
         <v>  GRAPH,    // Keyword `graph`    </v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="0" t="str">
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="0" t="str">
         <f aca="false">"%%]"</f>
         <v>%%]</v>
       </c>
-      <c r="B112" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="C112" s="0" t="s">
+      <c r="B113" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="C113" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="D112" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="E112" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B112,",    // ",C112," `",A112,"`    ",D112)</f>
+      <c r="D113" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="E113" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B113,",    // ",C113," `",A113,"`    ",D113)</f>
         <v>  GRAPH_END,    // Punctuation `%%]`    End of a graph literal</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="0" t="str">
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="str">
         <f aca="false">"[%%"</f>
         <v>[%%</v>
       </c>
-      <c r="B113" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="C113" s="0" t="s">
+      <c r="B114" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="C114" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="D113" s="0" t="s">
-        <v>181</v>
-      </c>
-      <c r="E113" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B113,",    // ",C113," `",A113,"`    ",D113)</f>
+      <c r="D114" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="E114" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B114,",    // ",C114," `",A114,"`    ",D114)</f>
         <v>  GRAPH_START,    // Punctuation `[%%`    Start of a graph literal</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="0" t="str">
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="str">
         <f aca="false">"&gt;"</f>
         <v>&gt;</v>
       </c>
-      <c r="B114" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="C114" s="0" t="s">
+      <c r="B115" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="C115" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="E114" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B114,",    // ",C114," `",A114,"`    ",D114)</f>
+      <c r="E115" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B115,",    // ",C115," `",A115,"`    ",D115)</f>
         <v>  GREATER_THAN,    // Operator `&gt;`    </v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="0" t="str">
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="str">
         <f aca="false">"&gt;="</f>
         <v>&gt;=</v>
       </c>
-      <c r="B115" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="C115" s="0" t="s">
+      <c r="B116" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="C116" s="0" t="s">
         <v>63</v>
-      </c>
-      <c r="E115" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B115,",    // ",C115," `",A115,"`    ",D115)</f>
-        <v>  GREATER_THAN_OR_EQUAL,    // Operator `&gt;=`    </v>
-      </c>
-    </row>
-    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="0" t="s">
-        <v>184</v>
-      </c>
-      <c r="B116" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="C116" s="0" t="s">
-        <v>185</v>
       </c>
       <c r="E116" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B116,",    // ",C116," `",A116,"`    ",D116)</f>
-        <v>  Identifier,    // Identifier `z_z1`    </v>
+        <v>  GREATER_THAN_OR_EQUAL,    // Operator `&gt;=`    </v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
         <v>186</v>
       </c>
-      <c r="B117" s="0" t="s">
+      <c r="B117" s="3" t="s">
         <v>187</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>7</v>
+        <v>187</v>
       </c>
       <c r="E117" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B117,",    // ",C117," `",A117,"`    ",D117)</f>
-        <v>  IF,    // Keyword `if`    </v>
+        <v>  Identifier,    // Identifier `z_z1`    </v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3038,7 +3043,7 @@
       </c>
       <c r="E118" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B118,",    // ",C118," `",A118,"`    ",D118)</f>
-        <v>  IMPORT,    // Keyword `import`    </v>
+        <v>  IF,    // Keyword `if`    </v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3053,7 +3058,7 @@
       </c>
       <c r="E119" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B119,",    // ",C119," `",A119,"`    ",D119)</f>
-        <v>  IN,    // Keyword `in`    </v>
+        <v>  IMPORT,    // Keyword `import`    </v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3068,7 +3073,7 @@
       </c>
       <c r="E120" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B120,",    // ",C120," `",A120,"`    ",D120)</f>
-        <v>  INSERT,    // Keyword `insert`    </v>
+        <v>  IN,    // Keyword `in`    </v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3083,70 +3088,70 @@
       </c>
       <c r="E121" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B121,",    // ",C121," `",A121,"`    ",D121)</f>
+        <v>  INSERT,    // Keyword `insert`    </v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="B122" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="C122" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E122" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B122,",    // ",C122," `",A122,"`    ",D122)</f>
         <v>  INSTANCE,    // Keyword `instance`    </v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="0" t="str">
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="str">
         <f aca="false">"0b101010"</f>
         <v>0b101010</v>
       </c>
-      <c r="B122" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="C122" s="0" t="s">
+      <c r="B123" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="C123" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E122" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B122,",    // ",C122," `",A122,"`    ",D122)</f>
+      <c r="E123" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B123,",    // ",C123," `",A123,"`    ",D123)</f>
         <v>  IntegerLiteral_Binary,    // Literal `0b101010`    </v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="0" t="str">
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="0" t="str">
         <f aca="false">"0"</f>
         <v>0</v>
       </c>
-      <c r="B123" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="C123" s="0" t="s">
+      <c r="B124" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="C124" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E123" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B123,",    // ",C123," `",A123,"`    ",D123)</f>
+      <c r="E124" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B124,",    // ",C124," `",A124,"`    ",D124)</f>
         <v>  IntegerLiteral_Decimal,    // Literal `0`    </v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="0" t="str">
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="0" t="str">
         <f aca="false">"0x12AB"</f>
         <v>0x12AB</v>
       </c>
-      <c r="B124" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="C124" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E124" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B124,",    // ",C124," `",A124,"`    ",D124)</f>
-        <v>  IntegerLiteral_Hex,    // Literal `0x12AB`    </v>
-      </c>
-    </row>
-    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="0" t="s">
-        <v>199</v>
-      </c>
       <c r="B125" s="0" t="s">
         <v>200</v>
       </c>
       <c r="C125" s="0" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E125" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B125,",    // ",C125," `",A125,"`    ",D125)</f>
-        <v>  INTERFACE,    // Keyword `interface`    </v>
+        <v>  IntegerLiteral_Hex,    // Literal `0x12AB`    </v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3161,7 +3166,7 @@
       </c>
       <c r="E126" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B126,",    // ",C126," `",A126,"`    ",D126)</f>
-        <v>  INTERSECTION,    // Keyword `intersection`    </v>
+        <v>  INTERFACE,    // Keyword `interface`    </v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3176,7 +3181,7 @@
       </c>
       <c r="E127" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B127,",    // ",C127," `",A127,"`    ",D127)</f>
-        <v>  IS,    // Keyword `is`    </v>
+        <v>  INTERSECTION,    // Keyword `intersection`    </v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3191,133 +3196,133 @@
       </c>
       <c r="E128" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B128,",    // ",C128," `",A128,"`    ",D128)</f>
+        <v>  IS,    // Keyword `is`    </v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="B129" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="C129" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E129" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B129,",    // ",C129," `",A129,"`    ",D129)</f>
         <v>  ISNOT,    // Keyword `isnot`    </v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="0" t="str">
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="0" t="str">
         <f aca="false">"{"</f>
         <v>{</v>
       </c>
-      <c r="B129" s="0" t="s">
-        <v>207</v>
-      </c>
-      <c r="C129" s="0" t="s">
+      <c r="B130" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="C130" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="E129" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B129,",    // ",C129," `",A129,"`    ",D129)</f>
+      <c r="E130" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B130,",    // ",C130," `",A130,"`    ",D130)</f>
         <v>  LEFT_BRACE,    // Punctuation `{`    </v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="0" t="str">
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="0" t="str">
         <f aca="false">"["</f>
         <v>[</v>
       </c>
-      <c r="B130" s="0" t="s">
-        <v>208</v>
-      </c>
-      <c r="C130" s="0" t="s">
+      <c r="B131" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="C131" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="E130" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B130,",    // ",C130," `",A130,"`    ",D130)</f>
+      <c r="E131" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B131,",    // ",C131," `",A131,"`    ",D131)</f>
         <v>  LEFT_BRACKET,    // Punctuation `[`    </v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="0" t="str">
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="0" t="str">
         <f aca="false">"("</f>
         <v>(</v>
       </c>
-      <c r="B131" s="0" t="s">
-        <v>209</v>
-      </c>
-      <c r="C131" s="0" t="s">
+      <c r="B132" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="C132" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="E131" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B131,",    // ",C131," `",A131,"`    ",D131)</f>
+      <c r="E132" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B132,",    // ",C132," `",A132,"`    ",D132)</f>
         <v>  LEFT_PARENTHESIS,    // Punctuation `(`    </v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="0" t="str">
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="0" t="str">
         <f aca="false">"&lt;"</f>
         <v>&lt;</v>
       </c>
-      <c r="B132" s="0" t="s">
-        <v>210</v>
-      </c>
-      <c r="C132" s="0" t="s">
+      <c r="B133" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="C133" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="E132" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B132,",    // ",C132," `",A132,"`    ",D132)</f>
+      <c r="E133" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B133,",    // ",C133," `",A133,"`    ",D133)</f>
         <v>  LESS_THAN,    // Operator `&lt;`    </v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="0" t="str">
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="0" t="str">
         <f aca="false">"&lt;="</f>
         <v>&lt;=</v>
       </c>
-      <c r="B133" s="0" t="s">
-        <v>211</v>
-      </c>
-      <c r="C133" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="E133" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B133,",    // ",C133," `",A133,"`    ",D133)</f>
-        <v>  LESS_THAN_OR_EQUAL,    // Operator `&lt;=`    </v>
-      </c>
-    </row>
-    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="0" t="s">
-        <v>212</v>
-      </c>
       <c r="B134" s="0" t="s">
         <v>213</v>
       </c>
       <c r="C134" s="0" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="E134" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B134,",    // ",C134," `",A134,"`    ",D134)</f>
+        <v>  LESS_THAN_OR_EQUAL,    // Operator `&lt;=`    </v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="B135" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="C135" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E135" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B135,",    // ",C135," `",A135,"`    ",D135)</f>
         <v>  LET,    // Keyword `let`    </v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="0" t="str">
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="0" t="str">
         <f aca="false">"@| ... |"</f>
         <v>@| ... |</v>
       </c>
-      <c r="B135" s="0" t="s">
-        <v>214</v>
-      </c>
-      <c r="C135" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E135" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B135,",    // ",C135," `",A135,"`    ",D135)</f>
-        <v>  LocationLiteral,    // Literal `@| ... |`    </v>
-      </c>
-    </row>
-    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="0" t="s">
-        <v>215</v>
-      </c>
       <c r="B136" s="0" t="s">
         <v>216</v>
       </c>
       <c r="C136" s="0" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E136" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B136,",    // ",C136," `",A136,"`    ",D136)</f>
-        <v>  MATCH,    // Keyword `match`    </v>
+        <v>  LocationLiteral,    // Literal `@| ... |`    </v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3328,45 +3333,45 @@
         <v>218</v>
       </c>
       <c r="C137" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="D137" s="0" t="s">
-        <v>219</v>
+        <v>7</v>
       </c>
       <c r="E137" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B137,",    // ",C137," `",A137,"`    ",D137)</f>
+        <v>  MATCH,    // Keyword `match`    </v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="B138" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="C138" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="D138" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="E138" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B138,",    // ",C138," `",A138,"`    ",D138)</f>
         <v>  MINUS,    // Operator `-`    Subtraction (infix); Negation (prefix)</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="0" t="str">
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="0" t="str">
         <f aca="false">"-="</f>
         <v>-=</v>
       </c>
-      <c r="B138" s="0" t="s">
-        <v>220</v>
-      </c>
-      <c r="C138" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="E138" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B138,",    // ",C138," `",A138,"`    ",D138)</f>
-        <v>  MINUS_EQUALS,    // Operator `-=`    </v>
-      </c>
-    </row>
-    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="0" t="s">
-        <v>221</v>
-      </c>
       <c r="B139" s="0" t="s">
         <v>222</v>
       </c>
       <c r="C139" s="0" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="E139" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B139,",    // ",C139," `",A139,"`    ",D139)</f>
-        <v>  MOD,    // Keyword `mod`    </v>
+        <v>  MINUS_EQUALS,    // Operator `-=`    </v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3381,7 +3386,7 @@
       </c>
       <c r="E140" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B140,",    // ",C140," `",A140,"`    ",D140)</f>
-        <v>  MODULE,    // Keyword `module`    </v>
+        <v>  MOD,    // Keyword `mod`    </v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3396,7 +3401,7 @@
       </c>
       <c r="E141" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B141,",    // ",C141," `",A141,"`    ",D141)</f>
-        <v>  NAMESPACE,    // Keyword `namespace`    </v>
+        <v>  MODULE,    // Keyword `module`    </v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3411,69 +3416,69 @@
       </c>
       <c r="E142" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B142,",    // ",C142," `",A142,"`    ",D142)</f>
+        <v>  NAMESPACE,    // Keyword `namespace`    </v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="B143" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="C143" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E143" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B143,",    // ",C143," `",A143,"`    ",D143)</f>
         <v>  NOT,    // Keyword `not`    </v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="0" t="str">
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="0" t="str">
         <f aca="false">"&lt;&gt;"</f>
         <v>&lt;&gt;</v>
       </c>
-      <c r="B143" s="0" t="s">
-        <v>229</v>
-      </c>
-      <c r="C143" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="E143" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B143,",    // ",C143," `",A143,"`    ",D143)</f>
-        <v>  NOT_EQUAL_TO,    // Operator `&lt;&gt;`    </v>
-      </c>
-    </row>
-    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="0" t="s">
-        <v>230</v>
-      </c>
       <c r="B144" s="0" t="s">
         <v>231</v>
       </c>
       <c r="C144" s="0" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="E144" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B144,",    // ",C144," `",A144,"`    ",D144)</f>
+        <v>  NOT_EQUAL_TO,    // Operator `&lt;&gt;`    </v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="B145" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="C145" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E145" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B145,",    // ",C145," `",A145,"`    ",D145)</f>
         <v>  NOTIN,    // Keyword `notin`    </v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="0" t="str">
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="0" t="str">
         <f aca="false">"123.45"</f>
         <v>123.45</v>
       </c>
-      <c r="B145" s="0" t="s">
-        <v>232</v>
-      </c>
-      <c r="C145" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E145" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B145,",    // ",C145," `",A145,"`    ",D145)</f>
-        <v>  NumberLiteral,    // Literal `123.45`    </v>
-      </c>
-    </row>
-    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="0" t="s">
-        <v>233</v>
-      </c>
       <c r="B146" s="0" t="s">
         <v>234</v>
       </c>
       <c r="C146" s="0" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E146" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B146,",    // ",C146," `",A146,"`    ",D146)</f>
-        <v>  OBJECT,    // Keyword `object`    </v>
+        <v>  NumberLiteral,    // Literal `123.45`    </v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3488,7 +3493,7 @@
       </c>
       <c r="E147" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B147,",    // ",C147," `",A147,"`    ",D147)</f>
-        <v>  OR,    // Keyword `or`    </v>
+        <v>  OBJECT,    // Keyword `object`    </v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3503,235 +3508,235 @@
       </c>
       <c r="E148" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B148,",    // ",C148," `",A148,"`    ",D148)</f>
+        <v>  OR,    // Keyword `or`    </v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="B149" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="C149" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E149" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B149,",    // ",C149," `",A149,"`    ",D149)</f>
         <v>  PACKAGE,    // Keyword `package`    </v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="0" t="str">
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="0" t="str">
         <f aca="false">"%"</f>
         <v>%</v>
       </c>
-      <c r="B149" s="0" t="s">
-        <v>239</v>
-      </c>
-      <c r="C149" s="0" t="s">
+      <c r="B150" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="C150" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="E149" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B149,",    // ",C149," `",A149,"`    ",D149)</f>
+      <c r="E150" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B150,",    // ",C150," `",A150,"`    ",D150)</f>
         <v>  PERCENT,    // Operator `%`    </v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="0" t="str">
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="0" t="str">
         <f aca="false">"+"</f>
         <v>+</v>
       </c>
-      <c r="B150" s="0" t="s">
-        <v>240</v>
-      </c>
-      <c r="C150" s="0" t="s">
+      <c r="B151" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="C151" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="E150" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B150,",    // ",C150," `",A150,"`    ",D150)</f>
+      <c r="E151" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B151,",    // ",C151," `",A151,"`    ",D151)</f>
         <v>  PLUS,    // Operator `+`    </v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="0" t="str">
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="0" t="str">
         <f aca="false">"+="</f>
         <v>+=</v>
       </c>
-      <c r="B151" s="0" t="s">
-        <v>241</v>
-      </c>
-      <c r="C151" s="0" t="s">
+      <c r="B152" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="C152" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="E151" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B151,",    // ",C151," `",A151,"`    ",D151)</f>
+      <c r="E152" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B152,",    // ",C152," `",A152,"`    ",D152)</f>
         <v>  PLUS_EQUALS,    // Operator `+=`    </v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="0" t="str">
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="0" t="str">
         <f aca="false">"^"</f>
         <v>^</v>
       </c>
-      <c r="B152" s="0" t="s">
-        <v>242</v>
-      </c>
-      <c r="C152" s="0" t="s">
+      <c r="B153" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="C153" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="E152" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B152,",    // ",C152," `",A152,"`    ",D152)</f>
+      <c r="E153" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B153,",    // ",C153," `",A153,"`    ",D153)</f>
         <v>  POWER,    // Operator `^`    </v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="0" t="str">
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="0" t="str">
         <f aca="false">"^="</f>
         <v>^=</v>
       </c>
-      <c r="B153" s="0" t="s">
-        <v>243</v>
-      </c>
-      <c r="C153" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="E153" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B153,",    // ",C153," `",A153,"`    ",D153)</f>
-        <v>  POWER_EQUALS,    // Operator `^=`    </v>
-      </c>
-    </row>
-    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="0" t="s">
-        <v>244</v>
-      </c>
       <c r="B154" s="0" t="s">
         <v>245</v>
       </c>
       <c r="C154" s="0" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="E154" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B154,",    // ",C154," `",A154,"`    ",D154)</f>
+        <v>  POWER_EQUALS,    // Operator `^=`    </v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="B155" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="C155" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E155" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B155,",    // ",C155," `",A155,"`    ",D155)</f>
         <v>  PROTOCOL,    // Keyword `protocol`    </v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="0" t="str">
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="0" t="str">
         <f aca="false">"?"</f>
         <v>?</v>
       </c>
-      <c r="B155" s="0" t="s">
-        <v>246</v>
-      </c>
-      <c r="C155" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="E155" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B155,",    // ",C155," `",A155,"`    ",D155)</f>
-        <v>  QUESTION,    // Punctuation `?`    </v>
-      </c>
-    </row>
-    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="0" t="s">
-        <v>247</v>
-      </c>
       <c r="B156" s="0" t="s">
         <v>248</v>
       </c>
       <c r="C156" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="D156" s="0" t="s">
-        <v>249</v>
+        <v>109</v>
       </c>
       <c r="E156" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B156,",    // ",C156," `",A156,"`    ",D156)</f>
-        <v>  QUESTION_QUESTION,    // Operator `??`    Null coalescence</v>
+        <v>  QUESTION,    // Punctuation `?`    </v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="B157" s="0" t="s">
         <v>250</v>
       </c>
-      <c r="B157" s="0" t="s">
+      <c r="C157" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="D157" s="0" t="s">
         <v>251</v>
-      </c>
-      <c r="C157" s="0" t="s">
-        <v>7</v>
       </c>
       <c r="E157" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B157,",    // ",C157," `",A157,"`    ",D157)</f>
+        <v>  QUESTION_QUESTION,    // Operator `??`    Null coalescence</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="B158" s="0" t="s">
+        <v>253</v>
+      </c>
+      <c r="C158" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E158" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B158,",    // ",C158," `",A158,"`    ",D158)</f>
         <v>  RAISE,    // Keyword `raise`    </v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="0" t="str">
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="0" t="str">
         <f aca="false">"..&lt;"</f>
         <v>..&lt;</v>
       </c>
-      <c r="B158" s="0" t="s">
-        <v>252</v>
-      </c>
-      <c r="C158" s="0" t="s">
+      <c r="B159" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="C159" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="D158" s="0" t="s">
-        <v>253</v>
-      </c>
-      <c r="E158" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B158,",    // ",C158," `",A158,"`    ",D158)</f>
+      <c r="D159" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="E159" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B159,",    // ",C159," `",A159,"`    ",D159)</f>
         <v>  RANGE_EXCLUSIVE,    // Operator `..&lt;`    Range from lower inclusive to upper exclusive</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="0" t="str">
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="0" t="str">
         <f aca="false">".."</f>
         <v>..</v>
       </c>
-      <c r="B159" s="0" t="s">
-        <v>254</v>
-      </c>
-      <c r="C159" s="0" t="s">
+      <c r="B160" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="C160" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="D159" s="0" t="s">
-        <v>255</v>
-      </c>
-      <c r="E159" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B159,",    // ",C159," `",A159,"`    ",D159)</f>
-        <v>  RANGE_INCLUSIVE,    // Operator `..`    Range from lower to upper inclusive</v>
-      </c>
-    </row>
-    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="0" t="s">
-        <v>256</v>
-      </c>
-      <c r="B160" s="0" t="s">
+      <c r="D160" s="0" t="s">
         <v>257</v>
-      </c>
-      <c r="C160" s="0" t="s">
-        <v>7</v>
       </c>
       <c r="E160" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B160,",    // ",C160," `",A160,"`    ",D160)</f>
+        <v>  RANGE_INCLUSIVE,    // Operator `..`    Range from lower to upper inclusive</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="B161" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="C161" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E161" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B161,",    // ",C161," `",A161,"`    ",D161)</f>
         <v>  REGARDLESS,    // Keyword `regardless`    </v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="0" t="str">
+    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="0" t="str">
         <f aca="false">"~/ ... /igm"</f>
         <v>~/ ... /igm</v>
       </c>
-      <c r="B161" s="0" t="s">
-        <v>258</v>
-      </c>
-      <c r="C161" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E161" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B161,",    // ",C161," `",A161,"`    ",D161)</f>
-        <v>  RegularExpressionLiteral,    // Literal `~/ ... /igm`    </v>
-      </c>
-    </row>
-    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="0" t="s">
-        <v>259</v>
-      </c>
       <c r="B162" s="0" t="s">
         <v>260</v>
       </c>
       <c r="C162" s="0" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E162" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B162,",    // ",C162," `",A162,"`    ",D162)</f>
-        <v>  REPEAT,    // Keyword `repeat`    </v>
+        <v>  RegularExpressionLiteral,    // Literal `~/ ... /igm`    </v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3746,70 +3751,70 @@
       </c>
       <c r="E163" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B163,",    // ",C163," `",A163,"`    ",D163)</f>
+        <v>  REPEAT,    // Keyword `repeat`    </v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="B164" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="C164" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E164" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B164,",    // ",C164," `",A164,"`    ",D164)</f>
         <v>  RETURN,    // Keyword `return`    </v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="0" t="str">
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="0" t="str">
         <f aca="false">"}"</f>
         <v>}</v>
       </c>
-      <c r="B164" s="0" t="s">
-        <v>263</v>
-      </c>
-      <c r="C164" s="0" t="s">
+      <c r="B165" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="C165" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="E164" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B164,",    // ",C164," `",A164,"`    ",D164)</f>
+      <c r="E165" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B165,",    // ",C165," `",A165,"`    ",D165)</f>
         <v>  RIGHT_BRACE,    // Punctuation `}`    </v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="0" t="str">
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="0" t="str">
         <f aca="false">"]"</f>
         <v>]</v>
       </c>
-      <c r="B165" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="C165" s="0" t="s">
+      <c r="B166" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="C166" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="E165" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B165,",    // ",C165," `",A165,"`    ",D165)</f>
+      <c r="E166" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B166,",    // ",C166," `",A166,"`    ",D166)</f>
         <v>  RIGHT_BRACKET,    // Punctuation `]`    </v>
       </c>
     </row>
-    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="0" t="str">
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="0" t="str">
         <f aca="false">")"</f>
         <v>)</v>
       </c>
-      <c r="B166" s="0" t="s">
-        <v>265</v>
-      </c>
-      <c r="C166" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="E166" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B166,",    // ",C166," `",A166,"`    ",D166)</f>
-        <v>  RIGHT_PARENTHESIS,    // Punctuation `)`    </v>
-      </c>
-    </row>
-    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="0" t="s">
-        <v>266</v>
-      </c>
       <c r="B167" s="0" t="s">
         <v>267</v>
       </c>
       <c r="C167" s="0" t="s">
-        <v>7</v>
+        <v>109</v>
       </c>
       <c r="E167" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B167,",    // ",C167," `",A167,"`    ",D167)</f>
-        <v>  RULE,    // Keyword `rule`    </v>
+        <v>  RIGHT_PARENTHESIS,    // Punctuation `)`    </v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3824,7 +3829,7 @@
       </c>
       <c r="E168" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B168,",    // ",C168," `",A168,"`    ",D168)</f>
-        <v>  SAMPLING,    // Keyword `sampling`    </v>
+        <v>  RULE,    // Keyword `rule`    </v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3839,7 +3844,7 @@
       </c>
       <c r="E169" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B169,",    // ",C169," `",A169,"`    ",D169)</f>
-        <v>  SCENARIO,    // Keyword `scenario`    </v>
+        <v>  SAMPLING,    // Keyword `sampling`    </v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3854,7 +3859,7 @@
       </c>
       <c r="E170" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B170,",    // ",C170," `",A170,"`    ",D170)</f>
-        <v>  SELECT,    // Keyword `select`    </v>
+        <v>  SCENARIO,    // Keyword `scenario`    </v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3869,38 +3874,38 @@
       </c>
       <c r="E171" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B171,",    // ",C171," `",A171,"`    ",D171)</f>
+        <v>  SELECT,    // Keyword `select`    </v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="B172" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="C172" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E172" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B172,",    // ",C172," `",A172,"`    ",D172)</f>
         <v>  SELF,    // Keyword `self`    </v>
       </c>
     </row>
-    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="0" t="str">
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="0" t="str">
         <f aca="false">";"</f>
         <v>;</v>
       </c>
-      <c r="B172" s="0" t="s">
-        <v>276</v>
-      </c>
-      <c r="C172" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="E172" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B172,",    // ",C172," `",A172,"`    ",D172)</f>
-        <v>  SEMICOLON,    // Punctuation `;`    </v>
-      </c>
-    </row>
-    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="0" t="s">
-        <v>277</v>
-      </c>
       <c r="B173" s="0" t="s">
         <v>278</v>
       </c>
       <c r="C173" s="0" t="s">
-        <v>7</v>
+        <v>109</v>
       </c>
       <c r="E173" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B173,",    // ",C173," `",A173,"`    ",D173)</f>
-        <v>  SETUP,    // Keyword `setup`    </v>
+        <v>  SEMICOLON,    // Punctuation `;`    </v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3915,7 +3920,7 @@
       </c>
       <c r="E174" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B174,",    // ",C174," `",A174,"`    ",D174)</f>
-        <v>  SPECIFICATION,    // Keyword `specification`    </v>
+        <v>  SETUP,    // Keyword `setup`    </v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3930,7 +3935,7 @@
       </c>
       <c r="E175" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B175,",    // ",C175," `",A175,"`    ",D175)</f>
-        <v>  STRUCTURE,    // Keyword `structure`    </v>
+        <v>  SPECIFICATION,    // Keyword `specification`    </v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3945,236 +3950,236 @@
       </c>
       <c r="E176" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B176,",    // ",C176," `",A176,"`    ",D176)</f>
+        <v>  STRUCTURE,    // Keyword `structure`    </v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="B177" s="0" t="s">
+        <v>286</v>
+      </c>
+      <c r="C177" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E177" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B177,",    // ",C177," `",A177,"`    ",D177)</f>
         <v>  SYMBOL,    // Keyword `symbol`    </v>
       </c>
     </row>
-    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="0" t="str">
+    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="B178" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="C178" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="E178" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B178,",    // ",C178," `",A178,"`    ",D178)</f>
+        <v>  Tag,    // Tag `#abc_def`    </v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="0" t="str">
         <f aca="false">"{{{...}}}"</f>
         <v>{{{...}}}</v>
       </c>
-      <c r="B177" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="C177" s="0" t="s">
+      <c r="B179" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="C179" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E177" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B177,",    // ",C177," `",A177,"`    ",D177)</f>
+      <c r="E179" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B179,",    // ",C179," `",A179,"`    ",D179)</f>
         <v>  TemplateLiteral,    // Literal `{{{...}}}`    </v>
       </c>
     </row>
-    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="0" t="s">
-        <v>286</v>
-      </c>
-      <c r="B178" s="0" t="s">
-        <v>287</v>
-      </c>
-      <c r="C178" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E178" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B178,",    // ",C178," `",A178,"`    ",D178)</f>
+    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="0" t="s">
+        <v>290</v>
+      </c>
+      <c r="B180" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="C180" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E180" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B180,",    // ",C180," `",A180,"`    ",D180)</f>
         <v>  TEST,    // Keyword `test`    </v>
       </c>
     </row>
-    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="0" t="str">
+    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="0" t="str">
         <f aca="false">"""..."""</f>
         <v>"..."</v>
       </c>
-      <c r="B179" s="0" t="s">
-        <v>288</v>
-      </c>
-      <c r="C179" s="0" t="s">
+      <c r="B181" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="C181" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E179" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B179,",    // ",C179," `",A179,"`    ",D179)</f>
+      <c r="E181" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B181,",    // ",C181," `",A181,"`    ",D181)</f>
         <v>  TextLiteral_DoubleQuoted,    // Literal `"..."`    </v>
       </c>
     </row>
-    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="0" t="str">
+    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="0" t="str">
         <f aca="false">"""""""..."""""""</f>
         <v>"""..."""</v>
       </c>
-      <c r="B180" s="0" t="s">
-        <v>289</v>
-      </c>
-      <c r="C180" s="0" t="s">
+      <c r="B182" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="C182" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E180" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B180,",    // ",C180," `",A180,"`    ",D180)</f>
+      <c r="E182" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B182,",    // ",C182," `",A182,"`    ",D182)</f>
         <v>  TextLiteral_DoubleQuotedMultiline,    // Literal `"""..."""`    </v>
       </c>
     </row>
-    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="0" t="str">
+    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="0" t="str">
         <f aca="false">"'...'"</f>
         <v>'...'</v>
       </c>
-      <c r="B181" s="0" t="s">
-        <v>290</v>
-      </c>
-      <c r="C181" s="0" t="s">
+      <c r="B183" s="0" t="s">
+        <v>294</v>
+      </c>
+      <c r="C183" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E181" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B181,",    // ",C181," `",A181,"`    ",D181)</f>
+      <c r="E183" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B183,",    // ",C183," `",A183,"`    ",D183)</f>
         <v>  TextLiteral_SingleQuoted,    // Literal `'...'`    </v>
       </c>
     </row>
-    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="0" t="str">
+    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="0" t="str">
         <f aca="false">"'''...'''"</f>
         <v>'''...'''</v>
       </c>
-      <c r="B182" s="0" t="s">
-        <v>291</v>
-      </c>
-      <c r="C182" s="0" t="s">
+      <c r="B184" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="C184" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E182" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B182,",    // ",C182," `",A182,"`    ",D182)</f>
+      <c r="E184" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B184,",    // ",C184," `",A184,"`    ",D184)</f>
         <v>  TextLiteral_SingleQuotedMultiline,    // Literal `'''...'''`    </v>
       </c>
     </row>
-    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="0" t="s">
-        <v>292</v>
-      </c>
-      <c r="B183" s="0" t="s">
-        <v>293</v>
-      </c>
-      <c r="C183" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E183" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B183,",    // ",C183," `",A183,"`    ",D183)</f>
+    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="0" t="s">
+        <v>296</v>
+      </c>
+      <c r="B185" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="C185" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E185" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B185,",    // ",C185," `",A185,"`    ",D185)</f>
         <v>  THEN,    // Keyword `then`    </v>
       </c>
     </row>
-    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="0" t="str">
+    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="0" t="str">
         <f aca="false">"~"</f>
         <v>~</v>
       </c>
-      <c r="B184" s="0" t="s">
-        <v>294</v>
-      </c>
-      <c r="C184" s="0" t="s">
+      <c r="B186" s="0" t="s">
+        <v>298</v>
+      </c>
+      <c r="C186" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="E184" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B184,",    // ",C184," `",A184,"`    ",D184)</f>
+      <c r="E186" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B186,",    // ",C186," `",A186,"`    ",D186)</f>
         <v>  TILDE,    // Operator `~`    </v>
       </c>
     </row>
-    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="0" t="str">
+    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="0" t="str">
         <f aca="false">"~="</f>
         <v>~=</v>
       </c>
-      <c r="B185" s="0" t="s">
-        <v>295</v>
-      </c>
-      <c r="C185" s="0" t="s">
+      <c r="B187" s="0" t="s">
+        <v>299</v>
+      </c>
+      <c r="C187" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="E185" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B185,",    // ",C185," `",A185,"`    ",D185)</f>
+      <c r="E187" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B187,",    // ",C187," `",A187,"`    ",D187)</f>
         <v>  TILDE_EQUALS,    // Operator `~=`    </v>
       </c>
     </row>
-    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A186" s="0" t="str">
+    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="0" t="str">
         <f aca="false">"*"</f>
         <v>*</v>
       </c>
-      <c r="B186" s="0" t="s">
-        <v>296</v>
-      </c>
-      <c r="C186" s="0" t="s">
+      <c r="B188" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="C188" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="E186" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B186,",    // ",C186," `",A186,"`    ",D186)</f>
+      <c r="E188" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B188,",    // ",C188," `",A188,"`    ",D188)</f>
         <v>  TIMES,    // Operator `*`    </v>
       </c>
     </row>
-    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A187" s="0" t="str">
+    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="0" t="str">
         <f aca="false">"*="</f>
         <v>*=</v>
       </c>
-      <c r="B187" s="0" t="s">
-        <v>297</v>
-      </c>
-      <c r="C187" s="0" t="s">
+      <c r="B189" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="C189" s="0" t="s">
         <v>63</v>
-      </c>
-      <c r="E187" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B187,",    // ",C187," `",A187,"`    ",D187)</f>
-        <v>  TIMES_EQUALS,    // Operator `*=`    </v>
-      </c>
-    </row>
-    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="0" t="s">
-        <v>298</v>
-      </c>
-      <c r="B188" s="0" t="s">
-        <v>299</v>
-      </c>
-      <c r="C188" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="D188" s="0" t="s">
-        <v>300</v>
-      </c>
-      <c r="E188" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B188,",    // ",C188," `",A188,"`    ",D188)</f>
-        <v>  TO_STRING,    // Operator `$`    Conversion to string (prefix)</v>
-      </c>
-    </row>
-    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A189" s="0" t="s">
-        <v>301</v>
-      </c>
-      <c r="B189" s="0" t="s">
-        <v>302</v>
-      </c>
-      <c r="C189" s="0" t="s">
-        <v>7</v>
       </c>
       <c r="E189" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B189,",    // ",C189," `",A189,"`    ",D189)</f>
-        <v>  TRANSFORM,    // Keyword `transform`    </v>
+        <v>  TIMES_EQUALS,    // Operator `*=`    </v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="B190" s="0" t="s">
         <v>303</v>
       </c>
-      <c r="B190" s="0" t="s">
+      <c r="C190" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="D190" s="0" t="s">
         <v>304</v>
-      </c>
-      <c r="C190" s="0" t="s">
-        <v>7</v>
       </c>
       <c r="E190" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B190,",    // ",C190," `",A190,"`    ",D190)</f>
-        <v>  TRANSLATE,    // Keyword `translate`    </v>
+        <v>  TO_STRING,    // Operator `$`    Conversion to string (prefix)</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A191" s="2" t="s">
+      <c r="A191" s="0" t="s">
         <v>305</v>
       </c>
-      <c r="B191" s="2" t="s">
+      <c r="B191" s="0" t="s">
         <v>306</v>
       </c>
       <c r="C191" s="0" t="s">
@@ -4182,7 +4187,7 @@
       </c>
       <c r="E191" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B191,",    // ",C191," `",A191,"`    ",D191)</f>
-        <v>  TRUE,    // Keyword `true`    </v>
+        <v>  TRANSFORM,    // Keyword `transform`    </v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4197,14 +4202,14 @@
       </c>
       <c r="E192" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B192,",    // ",C192," `",A192,"`    ",D192)</f>
-        <v>  TYPE,    // Keyword `type`    </v>
+        <v>  TRANSLATE,    // Keyword `translate`    </v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="0" t="s">
+      <c r="A193" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="B193" s="0" t="s">
+      <c r="B193" s="2" t="s">
         <v>310</v>
       </c>
       <c r="C193" s="0" t="s">
@@ -4212,7 +4217,7 @@
       </c>
       <c r="E193" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B193,",    // ",C193," `",A193,"`    ",D193)</f>
-        <v>  UNDEFINED,    // Keyword `undefined`    </v>
+        <v>  TRUE,    // Keyword `true`    </v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4227,7 +4232,7 @@
       </c>
       <c r="E194" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B194,",    // ",C194," `",A194,"`    ",D194)</f>
-        <v>  UNION,    // Keyword `union`    </v>
+        <v>  TYPE,    // Keyword `type`    </v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4242,7 +4247,7 @@
       </c>
       <c r="E195" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B195,",    // ",C195," `",A195,"`    ",D195)</f>
-        <v>  UNLESS,    // Keyword `unless`    </v>
+        <v>  UNDEFINED,    // Keyword `undefined`    </v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4257,7 +4262,7 @@
       </c>
       <c r="E196" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B196,",    // ",C196," `",A196,"`    ",D196)</f>
-        <v>  UNTIL,    // Keyword `until`    </v>
+        <v>  UNION,    // Keyword `union`    </v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4272,7 +4277,7 @@
       </c>
       <c r="E197" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B197,",    // ",C197," `",A197,"`    ",D197)</f>
-        <v>  UPDATE,    // Keyword `update`    </v>
+        <v>  UNLESS,    // Keyword `unless`    </v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4287,7 +4292,7 @@
       </c>
       <c r="E198" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B198,",    // ",C198," `",A198,"`    ",D198)</f>
-        <v>  USE,    // Keyword `use`    </v>
+        <v>  UNTIL,    // Keyword `until`    </v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4302,79 +4307,79 @@
       </c>
       <c r="E199" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B199,",    // ",C199," `",A199,"`    ",D199)</f>
-        <v>  UserDefinedKeyWord,    // Keyword `#abc`    </v>
+        <v>  UPDATE,    // Keyword `update`    </v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A200" s="0" t="str">
+      <c r="A200" s="0" t="s">
+        <v>323</v>
+      </c>
+      <c r="B200" s="0" t="s">
+        <v>324</v>
+      </c>
+      <c r="C200" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E200" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B200,",    // ",C200," `",A200,"`    ",D200)</f>
+        <v>  USE,    // Keyword `use`    </v>
+      </c>
+    </row>
+    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="0" t="str">
         <f aca="false">"#{...}"</f>
         <v>#{...}</v>
       </c>
-      <c r="B200" s="0" t="s">
-        <v>323</v>
-      </c>
-      <c r="C200" s="0" t="s">
+      <c r="B201" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="C201" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D200" s="0" t="s">
-        <v>324</v>
-      </c>
-      <c r="E200" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B200,",    // ",C200," `",A200,"`    ",D200)</f>
+      <c r="D201" s="0" t="s">
+        <v>326</v>
+      </c>
+      <c r="E201" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B201,",    // ",C201," `",A201,"`    ",D201)</f>
         <v>  UserDefinedLiteral_Braces,    // Literal `#{...}`    User-defined literal B</v>
       </c>
     </row>
-    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A201" s="0" t="str">
+    <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="0" t="str">
         <f aca="false">"#[...]"</f>
         <v>#[...]</v>
       </c>
-      <c r="B201" s="0" t="s">
-        <v>325</v>
-      </c>
-      <c r="C201" s="0" t="s">
+      <c r="B202" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="C202" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D201" s="0" t="s">
-        <v>326</v>
-      </c>
-      <c r="E201" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B201,",    // ",C201," `",A201,"`    ",D201)</f>
+      <c r="D202" s="0" t="s">
+        <v>328</v>
+      </c>
+      <c r="E202" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B202,",    // ",C202," `",A202,"`    ",D202)</f>
         <v>  UserDefinedLiteral_Brackets,    // Literal `#[...]`    User-defined literal A</v>
       </c>
     </row>
-    <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="0" t="str">
+    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="0" t="str">
         <f aca="false">"#/.../"</f>
         <v>#/.../</v>
       </c>
-      <c r="B202" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="C202" s="0" t="s">
+      <c r="B203" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="C203" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D202" s="0" t="s">
-        <v>328</v>
-      </c>
-      <c r="E202" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B202,",    // ",C202," `",A202,"`    ",D202)</f>
-        <v>  UserDefinedLiteral_Slashes,    // Literal `#/.../`    User-defined literal C</v>
-      </c>
-    </row>
-    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="0" t="s">
-        <v>329</v>
-      </c>
-      <c r="B203" s="0" t="s">
+      <c r="D203" s="0" t="s">
         <v>330</v>
-      </c>
-      <c r="C203" s="0" t="s">
-        <v>7</v>
       </c>
       <c r="E203" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B203,",    // ",C203," `",A203,"`    ",D203)</f>
-        <v>  VALUE,    // Keyword `value`    </v>
+        <v>  UserDefinedLiteral_Slashes,    // Literal `#/.../`    User-defined literal C</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4389,7 +4394,7 @@
       </c>
       <c r="E204" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B204,",    // ",C204," `",A204,"`    ",D204)</f>
-        <v>  VARIABLE,    // Keyword `variable`    </v>
+        <v>  VALUE,    // Keyword `value`    </v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4404,7 +4409,7 @@
       </c>
       <c r="E205" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B205,",    // ",C205," `",A205,"`    ",D205)</f>
-        <v>  VARIANT,    // Keyword `variant`    </v>
+        <v>  VARIABLE,    // Keyword `variable`    </v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4419,38 +4424,38 @@
       </c>
       <c r="E206" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B206,",    // ",C206," `",A206,"`    ",D206)</f>
+        <v>  VARIANT,    // Keyword `variant`    </v>
+      </c>
+    </row>
+    <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="0" t="s">
+        <v>337</v>
+      </c>
+      <c r="B207" s="0" t="s">
+        <v>338</v>
+      </c>
+      <c r="C207" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E207" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B207,",    // ",C207," `",A207,"`    ",D207)</f>
         <v>  VERSION,    // Keyword `version`    </v>
       </c>
     </row>
-    <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A207" s="0" t="str">
+    <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="0" t="str">
         <f aca="false">"2.3.4"</f>
         <v>2.3.4</v>
       </c>
-      <c r="B207" s="0" t="s">
-        <v>337</v>
-      </c>
-      <c r="C207" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E207" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B207,",    // ",C207," `",A207,"`    ",D207)</f>
-        <v>  VersionLiteral,    // Literal `2.3.4`    </v>
-      </c>
-    </row>
-    <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A208" s="0" t="s">
-        <v>338</v>
-      </c>
       <c r="B208" s="0" t="s">
         <v>339</v>
       </c>
       <c r="C208" s="0" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E208" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B208,",    // ",C208," `",A208,"`    ",D208)</f>
-        <v>  VERTEX,    // Keyword `vertex`    </v>
+        <v>  VersionLiteral,    // Literal `2.3.4`    </v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4465,7 +4470,7 @@
       </c>
       <c r="E209" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B209,",    // ",C209," `",A209,"`    ",D209)</f>
-        <v>  WHEN,    // Keyword `when`    </v>
+        <v>  VERTEX,    // Keyword `vertex`    </v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4480,7 +4485,7 @@
       </c>
       <c r="E210" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B210,",    // ",C210," `",A210,"`    ",D210)</f>
-        <v>  WHERE,    // Keyword `where`    </v>
+        <v>  WHEN,    // Keyword `when`    </v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4495,7 +4500,7 @@
       </c>
       <c r="E211" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B211,",    // ",C211," `",A211,"`    ",D211)</f>
-        <v>  WHILE,    // Keyword `while`    </v>
+        <v>  WHERE,    // Keyword `where`    </v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4510,7 +4515,7 @@
       </c>
       <c r="E212" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B212,",    // ",C212," `",A212,"`    ",D212)</f>
-        <v>  WITH,    // Keyword `with`    </v>
+        <v>  WHILE,    // Keyword `while`    </v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4525,7 +4530,7 @@
       </c>
       <c r="E213" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B213,",    // ",C213," `",A213,"`    ",D213)</f>
-        <v>  XOR,    // Keyword `xor`    </v>
+        <v>  WITH,    // Keyword `with`    </v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4540,6 +4545,21 @@
       </c>
       <c r="E214" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B214,",    // ",C214," `",A214,"`    ",D214)</f>
+        <v>  XOR,    // Keyword `xor`    </v>
+      </c>
+    </row>
+    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A215" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="B215" s="0" t="s">
+        <v>353</v>
+      </c>
+      <c r="C215" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E215" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B215,",    // ",C215," `",A215,"`    ",D215)</f>
         <v>  YIELD,    // Keyword `yield`    </v>
       </c>
     </row>

</xml_diff>

<commit_message>
* Revised tag concept to allow user-defined tags that look like identifiers.
</commit_message>
<xml_diff>
--- a/barlom-language/lexer/doc/TokenTypes.xlsx
+++ b/barlom-language/lexer/doc/TokenTypes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="352">
   <si>
     <t>Token Text</t>
   </si>
@@ -875,12 +875,6 @@
   </si>
   <si>
     <t>STRUCTURE</t>
-  </si>
-  <si>
-    <t>symbol</t>
-  </si>
-  <si>
-    <t>SYMBOL</t>
   </si>
   <si>
     <t>#abc_def</t>
@@ -1204,19 +1198,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E215"/>
+  <dimension ref="A1:E214"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A165" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A177" activeCellId="0" sqref="A177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.719387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.8877551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="74.6479591836735"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.3112244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="73.8418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1248,7 +1243,7 @@
       </c>
       <c r="E2" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B2,",    // ",C2," `",A2,"`    ",D2)</f>
-        <v>  AFTER,    // Keyword `after`    </v>
+        <v>AFTER,    // Keyword `after`</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1263,7 +1258,7 @@
       </c>
       <c r="E3" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B3,",    // ",C3," `",A3,"`    ",D3)</f>
-        <v>  ALIAS,    // Keyword `alias`    </v>
+        <v>ALIAS,    // Keyword `alias`</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1278,7 +1273,7 @@
       </c>
       <c r="E4" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B4,",    // ",C4," `",A4,"`    ",D4)</f>
-        <v>  AND,    // Keyword `and`    </v>
+        <v>AND,    // Keyword `and`</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1293,7 +1288,7 @@
       </c>
       <c r="E5" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B5,",    // ",C5," `",A5,"`    ",D5)</f>
-        <v>  ANNOTATION,    // Keyword `annotation`    </v>
+        <v>ANNOTATION,    // Keyword `annotation`</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1309,7 +1304,7 @@
       </c>
       <c r="E6" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B6,",    // ",C6," `",A6,"`    ",D6)</f>
-        <v>  ANONYMOUS_LITERAL,    // Literal `_`    </v>
+        <v>ANONYMOUS_LITERAL,    // Literal `_`</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1324,7 +1319,7 @@
       </c>
       <c r="E7" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B7,",    // ",C7," `",A7,"`    ",D7)</f>
-        <v>  AROUND,    // Keyword `around`    </v>
+        <v>AROUND,    // Keyword `around`</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1340,7 +1335,7 @@
       </c>
       <c r="E8" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B8,",    // ",C8," `",A8,"`    ",D8)</f>
-        <v>  ARROW_COLON_COLON_LEFT,    // Arrow `&lt;::`    </v>
+        <v>ARROW_COLON_COLON_LEFT,    // Arrow `&lt;::`</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1356,7 +1351,7 @@
       </c>
       <c r="E9" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B9,",    // ",C9," `",A9,"`    ",D9)</f>
-        <v>  ARROW_COLON_COLON_LEFT_RIGHT,    // Arrow `&lt;::&gt;`    </v>
+        <v>ARROW_COLON_COLON_LEFT_RIGHT,    // Arrow `&lt;::&gt;`</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1372,7 +1367,7 @@
       </c>
       <c r="E10" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B10,",    // ",C10," `",A10,"`    ",D10)</f>
-        <v>  ARROW_COLON_COLON_RIGHT,    // Arrow `::&gt;`    </v>
+        <v>ARROW_COLON_COLON_RIGHT,    // Arrow `::&gt;`</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1388,7 +1383,7 @@
       </c>
       <c r="E11" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B11,",    // ",C11," `",A11,"`    ",D11)</f>
-        <v>  ARROW_COLON_LEFT,    // Arrow `&lt;:`    </v>
+        <v>ARROW_COLON_LEFT,    // Arrow `&lt;:`</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1404,7 +1399,7 @@
       </c>
       <c r="E12" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B12,",    // ",C12," `",A12,"`    ",D12)</f>
-        <v>  ARROW_COLON_LEFT_RIGHT,    // Arrow `&lt;:&gt;`    </v>
+        <v>ARROW_COLON_LEFT_RIGHT,    // Arrow `&lt;:&gt;`</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1420,7 +1415,7 @@
       </c>
       <c r="E13" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B13,",    // ",C13," `",A13,"`    ",D13)</f>
-        <v>  ARROW_COLON_RIGHT,    // Arrow `:&gt;`    </v>
+        <v>ARROW_COLON_RIGHT,    // Arrow `:&gt;`</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1436,7 +1431,7 @@
       </c>
       <c r="E14" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B14,",    // ",C14," `",A14,"`    ",D14)</f>
-        <v>  ARROW_DASH_DASH_DASH,    // Arrow `---`    </v>
+        <v>ARROW_DASH_DASH_DASH,    // Arrow `---`</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1452,7 +1447,7 @@
       </c>
       <c r="E15" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B15,",    // ",C15," `",A15,"`    ",D15)</f>
-        <v>  ARROW_DASH_DASH_DIAMOND_LEFT,    // Arrow `&lt;&gt;--`    </v>
+        <v>ARROW_DASH_DASH_DIAMOND_LEFT,    // Arrow `&lt;&gt;--`</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1468,7 +1463,7 @@
       </c>
       <c r="E16" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B16,",    // ",C16," `",A16,"`    ",D16)</f>
-        <v>  ARROW_DASH_DASH_DIAMOND_RIGHT,    // Arrow `--&lt;&gt;`    </v>
+        <v>ARROW_DASH_DASH_DIAMOND_RIGHT,    // Arrow `--&lt;&gt;`</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1484,7 +1479,7 @@
       </c>
       <c r="E17" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B17,",    // ",C17," `",A17,"`    ",D17)</f>
-        <v>  ARROW_DASH_DASH_DOUBLE_LEFT,    // Arrow `&lt;&lt;--`    </v>
+        <v>ARROW_DASH_DASH_DOUBLE_LEFT,    // Arrow `&lt;&lt;--`</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1500,7 +1495,7 @@
       </c>
       <c r="E18" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B18,",    // ",C18," `",A18,"`    ",D18)</f>
-        <v>  ARROW_DASH_DASH_DOUBLE_RIGHT,    // Arrow `--&gt;&gt;`    </v>
+        <v>ARROW_DASH_DASH_DOUBLE_RIGHT,    // Arrow `--&gt;&gt;`</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1516,7 +1511,7 @@
       </c>
       <c r="E19" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B19,",    // ",C19," `",A19,"`    ",D19)</f>
-        <v>  ARROW_DASH_DASH_LEFT,    // Arrow `&lt;--`    </v>
+        <v>ARROW_DASH_DASH_LEFT,    // Arrow `&lt;--`</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1532,7 +1527,7 @@
       </c>
       <c r="E20" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B20,",    // ",C20," `",A20,"`    ",D20)</f>
-        <v>  ARROW_DASH_DASH_LEFT_RIGHT,    // Arrow `&lt;--&gt;`    </v>
+        <v>ARROW_DASH_DASH_LEFT_RIGHT,    // Arrow `&lt;--&gt;`</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1548,7 +1543,7 @@
       </c>
       <c r="E21" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B21,",    // ",C21," `",A21,"`    ",D21)</f>
-        <v>  ARROW_DASH_DASH_RIGHT,    // Arrow `--&gt;`    </v>
+        <v>ARROW_DASH_DASH_RIGHT,    // Arrow `--&gt;`</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1564,7 +1559,7 @@
       </c>
       <c r="E22" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B22,",    // ",C22," `",A22,"`    ",D22)</f>
-        <v>  ARROW_DASH_LEFT,    // Arrow `&lt;-`    </v>
+        <v>ARROW_DASH_LEFT,    // Arrow `&lt;-`</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1580,7 +1575,7 @@
       </c>
       <c r="E23" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B23,",    // ",C23," `",A23,"`    ",D23)</f>
-        <v>  ARROW_DASH_LEFT_RIGHT,    // Arrow `&lt;-&gt;`    </v>
+        <v>ARROW_DASH_LEFT_RIGHT,    // Arrow `&lt;-&gt;`</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1596,7 +1591,7 @@
       </c>
       <c r="E24" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B24,",    // ",C24," `",A24,"`    ",D24)</f>
-        <v>  ARROW_DASH_RIGHT,    // Arrow `-&gt;`    </v>
+        <v>ARROW_DASH_RIGHT,    // Arrow `-&gt;`</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1612,7 +1607,7 @@
       </c>
       <c r="E25" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B25,",    // ",C25," `",A25,"`    ",D25)</f>
-        <v>  ARROW_EQUAL_EQUAL_DIAMOND_LEFT,    // Arrow `&lt;&gt;==`    </v>
+        <v>ARROW_EQUAL_EQUAL_DIAMOND_LEFT,    // Arrow `&lt;&gt;==`</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1628,7 +1623,7 @@
       </c>
       <c r="E26" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B26,",    // ",C26," `",A26,"`    ",D26)</f>
-        <v>  ARROW_EQUAL_EQUAL_DIAMOND_RIGHT,    // Arrow `==&lt;&gt;`    </v>
+        <v>ARROW_EQUAL_EQUAL_DIAMOND_RIGHT,    // Arrow `==&lt;&gt;`</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1644,7 +1639,7 @@
       </c>
       <c r="E27" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B27,",    // ",C27," `",A27,"`    ",D27)</f>
-        <v>  ARROW_EQUAL_EQUAL_DOUBLE_LEFT,    // Arrow `&lt;&lt;==`    </v>
+        <v>ARROW_EQUAL_EQUAL_DOUBLE_LEFT,    // Arrow `&lt;&lt;==`</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1660,7 +1655,7 @@
       </c>
       <c r="E28" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B28,",    // ",C28," `",A28,"`    ",D28)</f>
-        <v>  ARROW_EQUAL_EQUAL_DOUBLE_RIGHT,    // Arrow `==&gt;&gt;`    </v>
+        <v>ARROW_EQUAL_EQUAL_DOUBLE_RIGHT,    // Arrow `==&gt;&gt;`</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1676,7 +1671,7 @@
       </c>
       <c r="E29" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B29,",    // ",C29," `",A29,"`    ",D29)</f>
-        <v>  ARROW_EQUAL_EQUAL_LEFT,    // Arrow `&lt;==`    </v>
+        <v>ARROW_EQUAL_EQUAL_LEFT,    // Arrow `&lt;==`</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1692,7 +1687,7 @@
       </c>
       <c r="E30" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B30,",    // ",C30," `",A30,"`    ",D30)</f>
-        <v>  ARROW_EQUAL_EQUAL_LEFT_RIGHT,    // Arrow `&lt;==&gt;`    </v>
+        <v>ARROW_EQUAL_EQUAL_LEFT_RIGHT,    // Arrow `&lt;==&gt;`</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1708,7 +1703,7 @@
       </c>
       <c r="E31" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B31,",    // ",C31," `",A31,"`    ",D31)</f>
-        <v>  ARROW_EQUAL_EQUAL_RIGHT,    // Arrow `==&gt;`    </v>
+        <v>ARROW_EQUAL_EQUAL_RIGHT,    // Arrow `==&gt;`</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1724,7 +1719,7 @@
       </c>
       <c r="E32" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B32,",    // ",C32," `",A32,"`    ",D32)</f>
-        <v>  ARROW_EQUAL_RIGHT,    // Arrow `=&gt;`    </v>
+        <v>ARROW_EQUAL_RIGHT,    // Arrow `=&gt;`</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1740,7 +1735,7 @@
       </c>
       <c r="E33" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B33,",    // ",C33," `",A33,"`    ",D33)</f>
-        <v>  ARROW_TILDE_LEFT,    // Arrow `&lt;~`    </v>
+        <v>ARROW_TILDE_LEFT,    // Arrow `&lt;~`</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1756,7 +1751,7 @@
       </c>
       <c r="E34" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B34,",    // ",C34," `",A34,"`    ",D34)</f>
-        <v>  ARROW_TILDE_LEFT_RIGHT,    // Arrow `&lt;~&gt;`    </v>
+        <v>ARROW_TILDE_LEFT_RIGHT,    // Arrow `&lt;~&gt;`</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1772,7 +1767,7 @@
       </c>
       <c r="E35" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B35,",    // ",C35," `",A35,"`    ",D35)</f>
-        <v>  ARROW_TILDE_RIGHT,    // Arrow `~&gt;`    </v>
+        <v>ARROW_TILDE_RIGHT,    // Arrow `~&gt;`</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1788,7 +1783,7 @@
       </c>
       <c r="E36" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B36,",    // ",C36," `",A36,"`    ",D36)</f>
-        <v>  ARROW_TILDE_TILDE_DIAMOND_LEFT,    // Arrow `&lt;&gt;~~`    </v>
+        <v>ARROW_TILDE_TILDE_DIAMOND_LEFT,    // Arrow `&lt;&gt;~~`</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1804,7 +1799,7 @@
       </c>
       <c r="E37" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B37,",    // ",C37," `",A37,"`    ",D37)</f>
-        <v>  ARROW_TILDE_TILDE_DIAMOND_RIGHT,    // Arrow `~~&lt;&gt;`    </v>
+        <v>ARROW_TILDE_TILDE_DIAMOND_RIGHT,    // Arrow `~~&lt;&gt;`</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1820,7 +1815,7 @@
       </c>
       <c r="E38" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B38,",    // ",C38," `",A38,"`    ",D38)</f>
-        <v>  ARROW_TILDE_TILDE_DOUBLE_LEFT,    // Arrow `&lt;&lt;~~`    </v>
+        <v>ARROW_TILDE_TILDE_DOUBLE_LEFT,    // Arrow `&lt;&lt;~~`</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1836,7 +1831,7 @@
       </c>
       <c r="E39" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B39,",    // ",C39," `",A39,"`    ",D39)</f>
-        <v>  ARROW_TILDE_TILDE_DOUBLE_RIGHT,    // Arrow `~~&gt;&gt;`    </v>
+        <v>ARROW_TILDE_TILDE_DOUBLE_RIGHT,    // Arrow `~~&gt;&gt;`</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1852,7 +1847,7 @@
       </c>
       <c r="E40" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B40,",    // ",C40," `",A40,"`    ",D40)</f>
-        <v>  ARROW_TILDE_TILDE_LEFT,    // Arrow `&lt;~~`    </v>
+        <v>ARROW_TILDE_TILDE_LEFT,    // Arrow `&lt;~~`</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1868,7 +1863,7 @@
       </c>
       <c r="E41" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B41,",    // ",C41," `",A41,"`    ",D41)</f>
-        <v>  ARROW_TILDE_TILDE_LEFT_RIGHT,    // Arrow `&lt;~~&gt;`    </v>
+        <v>ARROW_TILDE_TILDE_LEFT_RIGHT,    // Arrow `&lt;~~&gt;`</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1884,7 +1879,7 @@
       </c>
       <c r="E42" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B42,",    // ",C42," `",A42,"`    ",D42)</f>
-        <v>  ARROW_TILDE_TILDE_RIGHT,    // Arrow `~~&gt;`    </v>
+        <v>ARROW_TILDE_TILDE_RIGHT,    // Arrow `~~&gt;`</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1900,7 +1895,7 @@
       </c>
       <c r="E43" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B43,",    // ",C43," `",A43,"`    ",D43)</f>
-        <v>  ARROW_TILDE_TILDE_TILDE,    // Arrow `~~~`    </v>
+        <v>ARROW_TILDE_TILDE_TILDE,    // Arrow `~~~`</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1915,7 +1910,7 @@
       </c>
       <c r="E44" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B44,",    // ",C44," `",A44,"`    ",D44)</f>
-        <v>  AS,    // Keyword `as`    </v>
+        <v>AS,    // Keyword `as`</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1930,7 +1925,7 @@
       </c>
       <c r="E45" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B45,",    // ",C45," `",A45,"`    ",D45)</f>
-        <v>  ASPECT,    // Keyword `aspect`    </v>
+        <v>ASPECT,    // Keyword `aspect`</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1945,7 +1940,7 @@
       </c>
       <c r="E46" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B46,",    // ",C46," `",A46,"`    ",D46)</f>
-        <v>  ASSERT,    // Keyword `assert`    </v>
+        <v>ASSERT,    // Keyword `assert`</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1960,7 +1955,7 @@
       </c>
       <c r="E47" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B47,",    // ",C47," `",A47,"`    ",D47)</f>
-        <v>  AT,    // Operator `@`    </v>
+        <v>AT,    // Operator `@`</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1975,7 +1970,7 @@
       </c>
       <c r="E48" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B48,",    // ",C48," `",A48,"`    ",D48)</f>
-        <v>  BEFORE,    // Keyword `before`    </v>
+        <v>BEFORE,    // Keyword `before`</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1990,7 +1985,7 @@
       </c>
       <c r="E49" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B49,",    // ",C49," `",A49,"`    ",D49)</f>
-        <v>  BEGIN,    // Keyword `begin`    </v>
+        <v>BEGIN,    // Keyword `begin`</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2005,7 +2000,7 @@
       </c>
       <c r="E50" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B50,",    // ",C50," `",A50,"`    ",D50)</f>
-        <v>  BEHAVIOR,    // Keyword `behavior`    </v>
+        <v>BEHAVIOR,    // Keyword `behavior`</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2023,7 +2018,7 @@
       </c>
       <c r="E51" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B51,",    // ",C51," `",A51,"`    ",D51)</f>
-        <v>  BITWISE_AND,    // Operator `~and~`    Bitwise AND</v>
+        <v>BITWISE_AND,    // Operator `~and~`    Bitwise AND</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2041,7 +2036,7 @@
       </c>
       <c r="E52" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B52,",    // ",C52," `",A52,"`    ",D52)</f>
-        <v>  BITWISE_NAND,    // Operator `~nand~`    Bitwise NAND</v>
+        <v>BITWISE_NAND,    // Operator `~nand~`    Bitwise NAND</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2059,7 +2054,7 @@
       </c>
       <c r="E53" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B53,",    // ",C53," `",A53,"`    ",D53)</f>
-        <v>  BITWISE_NOR,    // Operator `~nor~`    Bitwise NOR</v>
+        <v>BITWISE_NOR,    // Operator `~nor~`    Bitwise NOR</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2077,7 +2072,7 @@
       </c>
       <c r="E54" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B54,",    // ",C54," `",A54,"`    ",D54)</f>
-        <v>  BITWISE_NOT,    // Operator `~not~`    Bitwise NOT (prefix)</v>
+        <v>BITWISE_NOT,    // Operator `~not~`    Bitwise NOT (prefix)</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2095,7 +2090,7 @@
       </c>
       <c r="E55" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B55,",    // ",C55," `",A55,"`    ",D55)</f>
-        <v>  BITWISE_OR,    // Operator `~or~`    Bitwise OR</v>
+        <v>BITWISE_OR,    // Operator `~or~`    Bitwise OR</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2113,7 +2108,7 @@
       </c>
       <c r="E56" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B56,",    // ",C56," `",A56,"`    ",D56)</f>
-        <v>  BITWISE_SHIFT_LEFT,    // Operator `~shl~`    Bitwise SHIFT LEFT</v>
+        <v>BITWISE_SHIFT_LEFT,    // Operator `~shl~`    Bitwise SHIFT LEFT</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2131,7 +2126,7 @@
       </c>
       <c r="E57" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B57,",    // ",C57," `",A57,"`    ",D57)</f>
-        <v>  BITWISE_SHIFT_RIGHT,    // Operator `~shr~`    Bitwise SHIFT RIGHT (sign extend)</v>
+        <v>BITWISE_SHIFT_RIGHT,    // Operator `~shr~`    Bitwise SHIFT RIGHT (sign extend)</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2149,7 +2144,7 @@
       </c>
       <c r="E58" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B58,",    // ",C58," `",A58,"`    ",D58)</f>
-        <v>  BITWISE_XOR,    // Operator `~xor~`    Bitwise XOR</v>
+        <v>BITWISE_XOR,    // Operator `~xor~`    Bitwise XOR</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2167,7 +2162,7 @@
       </c>
       <c r="E59" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B59,",    // ",C59," `",A59,"`    ",D59)</f>
-        <v>  BITWISE_ZERO_SHIFT_RIGHT,    // Operator `~zshr~`    Bitwise SHIFT RIGHT (zero extend)</v>
+        <v>BITWISE_ZERO_SHIFT_RIGHT,    // Operator `~zshr~`    Bitwise SHIFT RIGHT (zero extend)</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2182,7 +2177,7 @@
       </c>
       <c r="E60" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B60,",    // ",C60," `",A60,"`    ",D60)</f>
-        <v>  CALL,    // Keyword `call`    </v>
+        <v>CALL,    // Keyword `call`</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2197,7 +2192,7 @@
       </c>
       <c r="E61" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B61,",    // ",C61," `",A61,"`    ",D61)</f>
-        <v>  CASE,    // Keyword `case`    </v>
+        <v>CASE,    // Keyword `case`</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2212,7 +2207,7 @@
       </c>
       <c r="E62" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B62,",    // ",C62," `",A62,"`    ",D62)</f>
-        <v>  CHECK,    // Keyword `check`    </v>
+        <v>CHECK,    // Keyword `check`</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2227,7 +2222,7 @@
       </c>
       <c r="E63" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B63,",    // ",C63," `",A63,"`    ",D63)</f>
-        <v>  CLASS,    // Keyword `class`    </v>
+        <v>CLASS,    // Keyword `class`</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2242,7 +2237,7 @@
       </c>
       <c r="E64" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B64,",    // ",C64," `",A64,"`    ",D64)</f>
-        <v>  CLEANUP,    // Keyword `cleanup`    </v>
+        <v>CLEANUP,    // Keyword `cleanup`</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2258,7 +2253,7 @@
       </c>
       <c r="E65" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B65,",    // ",C65," `",A65,"`    ",D65)</f>
-        <v>  CodeLiteral,    // Literal ``...``    </v>
+        <v>CodeLiteral,    // Literal ``...``</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2274,7 +2269,7 @@
       </c>
       <c r="E66" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B66,",    // ",C66," `",A66,"`    ",D66)</f>
-        <v>  COLON,    // Punctuation `:`    </v>
+        <v>COLON,    // Punctuation `:`</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2290,7 +2285,7 @@
       </c>
       <c r="E67" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B67,",    // ",C67," `",A67,"`    ",D67)</f>
-        <v>  COLON_COLON,    // Punctuation `::`    </v>
+        <v>COLON_COLON,    // Punctuation `::`</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2306,7 +2301,7 @@
       </c>
       <c r="E68" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B68,",    // ",C68," `",A68,"`    ",D68)</f>
-        <v>  COMMA,    // Punctuation `,`    </v>
+        <v>COMMA,    // Punctuation `,`</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2322,7 +2317,7 @@
       </c>
       <c r="E69" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B69,",    // ",C69," `",A69,"`    ",D69)</f>
-        <v>  COMPARE,    // Operator `&lt;=&gt;`    </v>
+        <v>COMPARE,    // Operator `&lt;=&gt;`</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2338,7 +2333,7 @@
       </c>
       <c r="E70" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B70,",    // ",C70," `",A70,"`    ",D70)</f>
-        <v>  CONCAT_EQUALS,    // Operator `&amp;=`    </v>
+        <v>CONCAT_EQUALS,    // Operator `&amp;=`</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2354,7 +2349,7 @@
       </c>
       <c r="E71" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B71,",    // ",C71," `",A71,"`    ",D71)</f>
-        <v>  CONCATENATE,    // Operator `&amp;`    </v>
+        <v>CONCATENATE,    // Operator `&amp;`</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2369,7 +2364,7 @@
       </c>
       <c r="E72" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B72,",    // ",C72," `",A72,"`    ",D72)</f>
-        <v>  CONSTANT,    // Keyword `constant`    </v>
+        <v>CONSTANT,    // Keyword `constant`</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2384,7 +2379,7 @@
       </c>
       <c r="E73" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B73,",    // ",C73," `",A73,"`    ",D73)</f>
-        <v>  CONTEXT,    // Keyword `context`    </v>
+        <v>CONTEXT,    // Keyword `context`</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2399,7 +2394,7 @@
       </c>
       <c r="E74" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B74,",    // ",C74," `",A74,"`    ",D74)</f>
-        <v>  DATA,    // Keyword `data`    </v>
+        <v>DATA,    // Keyword `data`</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2415,7 +2410,7 @@
       </c>
       <c r="E75" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B75,",    // ",C75," `",A75,"`    ",D75)</f>
-        <v>  DateTimeLiteral,    // Literal `$2016-12-31T12:01:14.001-05:00$`    </v>
+        <v>DateTimeLiteral,    // Literal `$2016-12-31T12:01:14.001-05:00$`</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2430,7 +2425,7 @@
       </c>
       <c r="E76" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B76,",    // ",C76," `",A76,"`    ",D76)</f>
-        <v>  DEFAULT,    // Keyword `default`    </v>
+        <v>DEFAULT,    // Keyword `default`</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2445,7 +2440,7 @@
       </c>
       <c r="E77" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B77,",    // ",C77," `",A77,"`    ",D77)</f>
-        <v>  DEFER,    // Keyword `defer`    </v>
+        <v>DEFER,    // Keyword `defer`</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2460,7 +2455,7 @@
       </c>
       <c r="E78" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B78,",    // ",C78," `",A78,"`    ",D78)</f>
-        <v>  DEFINE,    // Keyword `define`    </v>
+        <v>DEFINE,    // Keyword `define`</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2475,7 +2470,7 @@
       </c>
       <c r="E79" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B79,",    // ",C79," `",A79,"`    ",D79)</f>
-        <v>  DELETE,    // Keyword `delete`    </v>
+        <v>DELETE,    // Keyword `delete`</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2490,7 +2485,7 @@
       </c>
       <c r="E80" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B80,",    // ",C80," `",A80,"`    ",D80)</f>
-        <v>  DETECT,    // Keyword `detect`    </v>
+        <v>DETECT,    // Keyword `detect`</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2505,7 +2500,7 @@
       </c>
       <c r="E81" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B81,",    // ",C81," `",A81,"`    ",D81)</f>
-        <v>  DIV,    // Keyword `div`    </v>
+        <v>DIV,    // Keyword `div`</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2521,7 +2516,7 @@
       </c>
       <c r="E82" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B82,",    // ",C82," `",A82,"`    ",D82)</f>
-        <v>  DIVIDE_EQUALS,    // Operator `/=`    </v>
+        <v>DIVIDE_EQUALS,    // Operator `/=`</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2537,7 +2532,7 @@
       </c>
       <c r="E83" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B83,",    // ",C83," `",A83,"`    ",D83)</f>
-        <v>  DIVIDED_BY,    // Operator `/`    </v>
+        <v>DIVIDED_BY,    // Operator `/`</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2552,7 +2547,7 @@
       </c>
       <c r="E84" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B84,",    // ",C84," `",A84,"`    ",D84)</f>
-        <v>  DO,    // Keyword `do`    </v>
+        <v>DO,    // Keyword `do`</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2571,7 +2566,7 @@
       </c>
       <c r="E85" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B85,",    // ",C85," `",A85,"`    ",D85)</f>
-        <v>  Documentation,    // Documentation `/*...*/`    Annotation documentation for an element</v>
+        <v>Documentation,    // Documentation `/*...*/`    Annotation documentation for an element</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2587,7 +2582,7 @@
       </c>
       <c r="E86" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B86,",    // ",C86," `",A86,"`    ",D86)</f>
-        <v>  DOT,    // Punctuation `.`    </v>
+        <v>DOT,    // Punctuation `.`</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2603,7 +2598,7 @@
       </c>
       <c r="E87" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B87,",    // ",C87," `",A87,"`    ",D87)</f>
-        <v>  DOT_DOT_DOT,    // Punctuation `...`    </v>
+        <v>DOT_DOT_DOT,    // Punctuation `...`</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2618,7 +2613,7 @@
       </c>
       <c r="E88" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B88,",    // ",C88," `",A88,"`    ",D88)</f>
-        <v>  DOT_QUESTION,    // Punctuation `.?`    </v>
+        <v>DOT_QUESTION,    // Punctuation `.?`</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2633,7 +2628,7 @@
       </c>
       <c r="E89" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B89,",    // ",C89," `",A89,"`    ",D89)</f>
-        <v>  EDGE,    // Keyword `edge`    </v>
+        <v>EDGE,    // Keyword `edge`</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2648,7 +2643,7 @@
       </c>
       <c r="E90" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B90,",    // ",C90," `",A90,"`    ",D90)</f>
-        <v>  ELSE,    // Keyword `else`    </v>
+        <v>ELSE,    // Keyword `else`</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2663,7 +2658,7 @@
       </c>
       <c r="E91" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B91,",    // ",C91," `",A91,"`    ",D91)</f>
-        <v>  END,    // Keyword `end`    </v>
+        <v>END,    // Keyword `end`</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2678,7 +2673,7 @@
       </c>
       <c r="E92" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B92,",    // ",C92," `",A92,"`    ",D92)</f>
-        <v>  ENUMERATION,    // Keyword `enumeration`    </v>
+        <v>ENUMERATION,    // Keyword `enumeration`</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2694,7 +2689,7 @@
       </c>
       <c r="E93" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B93,",    // ",C93," `",A93,"`    ",D93)</f>
-        <v>  EQUALS,    // Operator `=`    </v>
+        <v>EQUALS,    // Operator `=`</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2709,7 +2704,7 @@
       </c>
       <c r="E94" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B94,",    // ",C94," `",A94,"`    ",D94)</f>
-        <v>  ERROR,    // Keyword `error`    </v>
+        <v>ERROR,    // Keyword `error`</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2721,7 +2716,7 @@
       </c>
       <c r="E95" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B95,",    // ",C95," `",A95,"`    ",D95)</f>
-        <v>  ErrorInvalidIdentifier,    // Error ``    </v>
+        <v>ErrorInvalidIdentifier,    // Error ``</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2733,7 +2728,7 @@
       </c>
       <c r="E96" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B96,",    // ",C96," `",A96,"`    ",D96)</f>
-        <v>  ErrorInvalidMultilineTextLiteral,    // Error ``    </v>
+        <v>ErrorInvalidMultilineTextLiteral,    // Error ``</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2745,7 +2740,7 @@
       </c>
       <c r="E97" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B97,",    // ",C97," `",A97,"`    ",D97)</f>
-        <v>  ErrorInvalidTextLiteral,    // Error ``    </v>
+        <v>ErrorInvalidTextLiteral,    // Error ``</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2757,7 +2752,7 @@
       </c>
       <c r="E98" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B98,",    // ",C98," `",A98,"`    ",D98)</f>
-        <v>  ErrorInvalidTimeLiteral,    // Error ``    </v>
+        <v>ErrorInvalidTimeLiteral,    // Error ``</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2769,7 +2764,7 @@
       </c>
       <c r="E99" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B99,",    // ",C99," `",A99,"`    ",D99)</f>
-        <v>  ErrorUnclosedBlockComment,    // Error ``    </v>
+        <v>ErrorUnclosedBlockComment,    // Error ``</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2781,7 +2776,7 @@
       </c>
       <c r="E100" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B100,",    // ",C100," `",A100,"`    ",D100)</f>
-        <v>  ErrorUnclosedCodeLiteral,    // Error ``    </v>
+        <v>ErrorUnclosedCodeLiteral,    // Error ``</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2793,7 +2788,7 @@
       </c>
       <c r="E101" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B101,",    // ",C101," `",A101,"`    ",D101)</f>
-        <v>  ErrorUnclosedLocationLiteral,    // Error ``    </v>
+        <v>ErrorUnclosedLocationLiteral,    // Error ``</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2805,7 +2800,7 @@
       </c>
       <c r="E102" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B102,",    // ",C102," `",A102,"`    ",D102)</f>
-        <v>  ErrorUnclosedRegularExpression,    // Error ``    </v>
+        <v>ErrorUnclosedRegularExpression,    // Error ``</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2817,7 +2812,7 @@
       </c>
       <c r="E103" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B103,",    // ",C103," `",A103,"`    ",D103)</f>
-        <v>  ErrorUnclosedTemplate,    // Error ``    </v>
+        <v>ErrorUnclosedTemplate,    // Error ``</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2829,7 +2824,7 @@
       </c>
       <c r="E104" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B104,",    // ",C104," `",A104,"`    ",D104)</f>
-        <v>  ErrorUnclosedTextLiteral,    // Error ``    </v>
+        <v>ErrorUnclosedTextLiteral,    // Error ``</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2841,7 +2836,7 @@
       </c>
       <c r="E105" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B105,",    // ",C105," `",A105,"`    ",D105)</f>
-        <v>  ErrorUnclosedTextLiteralMultiline,    // Error ``    </v>
+        <v>ErrorUnclosedTextLiteralMultiline,    // Error ``</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2853,7 +2848,7 @@
       </c>
       <c r="E106" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B106,",    // ",C106," `",A106,"`    ",D106)</f>
-        <v>  ErrorUnexpectedCharacter,    // Error ``    </v>
+        <v>ErrorUnexpectedCharacter,    // Error ``</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2868,7 +2863,7 @@
       </c>
       <c r="E107" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B107,",    // ",C107," `",A107,"`    ",D107)</f>
-        <v>  EXPECT,    // Keyword `expect`    </v>
+        <v>EXPECT,    // Keyword `expect`</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2883,7 +2878,7 @@
       </c>
       <c r="E108" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B108,",    // ",C108," `",A108,"`    ",D108)</f>
-        <v>  FALSE,    // Keyword `false`    </v>
+        <v>FALSE,    // Keyword `false`</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2898,7 +2893,7 @@
       </c>
       <c r="E109" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B109,",    // ",C109," `",A109,"`    ",D109)</f>
-        <v>  FOR,    // Keyword `for`    </v>
+        <v>FOR,    // Keyword `for`</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2913,7 +2908,7 @@
       </c>
       <c r="E110" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B110,",    // ",C110," `",A110,"`    ",D110)</f>
-        <v>  FUNCTION,    // Keyword `function`    </v>
+        <v>FUNCTION,    // Keyword `function`</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2928,7 +2923,7 @@
       </c>
       <c r="E111" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B111,",    // ",C111," `",A111,"`    ",D111)</f>
-        <v>  GIVEN,    // Keyword `given`    </v>
+        <v>GIVEN,    // Keyword `given`</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2943,7 +2938,7 @@
       </c>
       <c r="E112" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B112,",    // ",C112," `",A112,"`    ",D112)</f>
-        <v>  GRAPH,    // Keyword `graph`    </v>
+        <v>GRAPH,    // Keyword `graph`</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2962,7 +2957,7 @@
       </c>
       <c r="E113" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B113,",    // ",C113," `",A113,"`    ",D113)</f>
-        <v>  GRAPH_END,    // Punctuation `%%]`    End of a graph literal</v>
+        <v>GRAPH_END,    // Punctuation `%%]`    End of a graph literal</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2981,7 +2976,7 @@
       </c>
       <c r="E114" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B114,",    // ",C114," `",A114,"`    ",D114)</f>
-        <v>  GRAPH_START,    // Punctuation `[%%`    Start of a graph literal</v>
+        <v>GRAPH_START,    // Punctuation `[%%`    Start of a graph literal</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2997,7 +2992,7 @@
       </c>
       <c r="E115" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B115,",    // ",C115," `",A115,"`    ",D115)</f>
-        <v>  GREATER_THAN,    // Operator `&gt;`    </v>
+        <v>GREATER_THAN,    // Operator `&gt;`</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3013,7 +3008,7 @@
       </c>
       <c r="E116" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B116,",    // ",C116," `",A116,"`    ",D116)</f>
-        <v>  GREATER_THAN_OR_EQUAL,    // Operator `&gt;=`    </v>
+        <v>GREATER_THAN_OR_EQUAL,    // Operator `&gt;=`</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3028,7 +3023,7 @@
       </c>
       <c r="E117" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B117,",    // ",C117," `",A117,"`    ",D117)</f>
-        <v>  Identifier,    // Identifier `z_z1`    </v>
+        <v>Identifier,    // Identifier `z_z1`</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3043,7 +3038,7 @@
       </c>
       <c r="E118" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B118,",    // ",C118," `",A118,"`    ",D118)</f>
-        <v>  IF,    // Keyword `if`    </v>
+        <v>IF,    // Keyword `if`</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3058,7 +3053,7 @@
       </c>
       <c r="E119" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B119,",    // ",C119," `",A119,"`    ",D119)</f>
-        <v>  IMPORT,    // Keyword `import`    </v>
+        <v>IMPORT,    // Keyword `import`</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3073,7 +3068,7 @@
       </c>
       <c r="E120" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B120,",    // ",C120," `",A120,"`    ",D120)</f>
-        <v>  IN,    // Keyword `in`    </v>
+        <v>IN,    // Keyword `in`</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3088,7 +3083,7 @@
       </c>
       <c r="E121" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B121,",    // ",C121," `",A121,"`    ",D121)</f>
-        <v>  INSERT,    // Keyword `insert`    </v>
+        <v>INSERT,    // Keyword `insert`</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3103,7 +3098,7 @@
       </c>
       <c r="E122" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B122,",    // ",C122," `",A122,"`    ",D122)</f>
-        <v>  INSTANCE,    // Keyword `instance`    </v>
+        <v>INSTANCE,    // Keyword `instance`</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3119,7 +3114,7 @@
       </c>
       <c r="E123" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B123,",    // ",C123," `",A123,"`    ",D123)</f>
-        <v>  IntegerLiteral_Binary,    // Literal `0b101010`    </v>
+        <v>IntegerLiteral_Binary,    // Literal `0b101010`</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3135,7 +3130,7 @@
       </c>
       <c r="E124" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B124,",    // ",C124," `",A124,"`    ",D124)</f>
-        <v>  IntegerLiteral_Decimal,    // Literal `0`    </v>
+        <v>IntegerLiteral_Decimal,    // Literal `0`</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3151,7 +3146,7 @@
       </c>
       <c r="E125" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B125,",    // ",C125," `",A125,"`    ",D125)</f>
-        <v>  IntegerLiteral_Hex,    // Literal `0x12AB`    </v>
+        <v>IntegerLiteral_Hex,    // Literal `0x12AB`</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3166,7 +3161,7 @@
       </c>
       <c r="E126" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B126,",    // ",C126," `",A126,"`    ",D126)</f>
-        <v>  INTERFACE,    // Keyword `interface`    </v>
+        <v>INTERFACE,    // Keyword `interface`</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3181,7 +3176,7 @@
       </c>
       <c r="E127" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B127,",    // ",C127," `",A127,"`    ",D127)</f>
-        <v>  INTERSECTION,    // Keyword `intersection`    </v>
+        <v>INTERSECTION,    // Keyword `intersection`</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3196,7 +3191,7 @@
       </c>
       <c r="E128" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B128,",    // ",C128," `",A128,"`    ",D128)</f>
-        <v>  IS,    // Keyword `is`    </v>
+        <v>IS,    // Keyword `is`</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3211,7 +3206,7 @@
       </c>
       <c r="E129" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B129,",    // ",C129," `",A129,"`    ",D129)</f>
-        <v>  ISNOT,    // Keyword `isnot`    </v>
+        <v>ISNOT,    // Keyword `isnot`</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3227,7 +3222,7 @@
       </c>
       <c r="E130" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B130,",    // ",C130," `",A130,"`    ",D130)</f>
-        <v>  LEFT_BRACE,    // Punctuation `{`    </v>
+        <v>LEFT_BRACE,    // Punctuation `{`</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3243,7 +3238,7 @@
       </c>
       <c r="E131" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B131,",    // ",C131," `",A131,"`    ",D131)</f>
-        <v>  LEFT_BRACKET,    // Punctuation `[`    </v>
+        <v>LEFT_BRACKET,    // Punctuation `[`</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3259,7 +3254,7 @@
       </c>
       <c r="E132" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B132,",    // ",C132," `",A132,"`    ",D132)</f>
-        <v>  LEFT_PARENTHESIS,    // Punctuation `(`    </v>
+        <v>LEFT_PARENTHESIS,    // Punctuation `(`</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3275,7 +3270,7 @@
       </c>
       <c r="E133" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B133,",    // ",C133," `",A133,"`    ",D133)</f>
-        <v>  LESS_THAN,    // Operator `&lt;`    </v>
+        <v>LESS_THAN,    // Operator `&lt;`</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3291,7 +3286,7 @@
       </c>
       <c r="E134" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B134,",    // ",C134," `",A134,"`    ",D134)</f>
-        <v>  LESS_THAN_OR_EQUAL,    // Operator `&lt;=`    </v>
+        <v>LESS_THAN_OR_EQUAL,    // Operator `&lt;=`</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3306,7 +3301,7 @@
       </c>
       <c r="E135" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B135,",    // ",C135," `",A135,"`    ",D135)</f>
-        <v>  LET,    // Keyword `let`    </v>
+        <v>LET,    // Keyword `let`</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3322,7 +3317,7 @@
       </c>
       <c r="E136" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B136,",    // ",C136," `",A136,"`    ",D136)</f>
-        <v>  LocationLiteral,    // Literal `@| ... |`    </v>
+        <v>LocationLiteral,    // Literal `@| ... |`</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3337,7 +3332,7 @@
       </c>
       <c r="E137" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B137,",    // ",C137," `",A137,"`    ",D137)</f>
-        <v>  MATCH,    // Keyword `match`    </v>
+        <v>MATCH,    // Keyword `match`</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3355,7 +3350,7 @@
       </c>
       <c r="E138" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B138,",    // ",C138," `",A138,"`    ",D138)</f>
-        <v>  MINUS,    // Operator `-`    Subtraction (infix); Negation (prefix)</v>
+        <v>MINUS,    // Operator `-`    Subtraction (infix); Negation (prefix)</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3371,7 +3366,7 @@
       </c>
       <c r="E139" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B139,",    // ",C139," `",A139,"`    ",D139)</f>
-        <v>  MINUS_EQUALS,    // Operator `-=`    </v>
+        <v>MINUS_EQUALS,    // Operator `-=`</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3386,7 +3381,7 @@
       </c>
       <c r="E140" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B140,",    // ",C140," `",A140,"`    ",D140)</f>
-        <v>  MOD,    // Keyword `mod`    </v>
+        <v>MOD,    // Keyword `mod`</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3401,7 +3396,7 @@
       </c>
       <c r="E141" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B141,",    // ",C141," `",A141,"`    ",D141)</f>
-        <v>  MODULE,    // Keyword `module`    </v>
+        <v>MODULE,    // Keyword `module`</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3416,7 +3411,7 @@
       </c>
       <c r="E142" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B142,",    // ",C142," `",A142,"`    ",D142)</f>
-        <v>  NAMESPACE,    // Keyword `namespace`    </v>
+        <v>NAMESPACE,    // Keyword `namespace`</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3431,7 +3426,7 @@
       </c>
       <c r="E143" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B143,",    // ",C143," `",A143,"`    ",D143)</f>
-        <v>  NOT,    // Keyword `not`    </v>
+        <v>NOT,    // Keyword `not`</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3447,7 +3442,7 @@
       </c>
       <c r="E144" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B144,",    // ",C144," `",A144,"`    ",D144)</f>
-        <v>  NOT_EQUAL_TO,    // Operator `&lt;&gt;`    </v>
+        <v>NOT_EQUAL_TO,    // Operator `&lt;&gt;`</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3462,7 +3457,7 @@
       </c>
       <c r="E145" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B145,",    // ",C145," `",A145,"`    ",D145)</f>
-        <v>  NOTIN,    // Keyword `notin`    </v>
+        <v>NOTIN,    // Keyword `notin`</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3478,7 +3473,7 @@
       </c>
       <c r="E146" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B146,",    // ",C146," `",A146,"`    ",D146)</f>
-        <v>  NumberLiteral,    // Literal `123.45`    </v>
+        <v>NumberLiteral,    // Literal `123.45`</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3493,7 +3488,7 @@
       </c>
       <c r="E147" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B147,",    // ",C147," `",A147,"`    ",D147)</f>
-        <v>  OBJECT,    // Keyword `object`    </v>
+        <v>OBJECT,    // Keyword `object`</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3508,7 +3503,7 @@
       </c>
       <c r="E148" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B148,",    // ",C148," `",A148,"`    ",D148)</f>
-        <v>  OR,    // Keyword `or`    </v>
+        <v>OR,    // Keyword `or`</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3523,7 +3518,7 @@
       </c>
       <c r="E149" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B149,",    // ",C149," `",A149,"`    ",D149)</f>
-        <v>  PACKAGE,    // Keyword `package`    </v>
+        <v>PACKAGE,    // Keyword `package`</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3539,7 +3534,7 @@
       </c>
       <c r="E150" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B150,",    // ",C150," `",A150,"`    ",D150)</f>
-        <v>  PERCENT,    // Operator `%`    </v>
+        <v>PERCENT,    // Operator `%`</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3555,7 +3550,7 @@
       </c>
       <c r="E151" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B151,",    // ",C151," `",A151,"`    ",D151)</f>
-        <v>  PLUS,    // Operator `+`    </v>
+        <v>PLUS,    // Operator `+`</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3571,7 +3566,7 @@
       </c>
       <c r="E152" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B152,",    // ",C152," `",A152,"`    ",D152)</f>
-        <v>  PLUS_EQUALS,    // Operator `+=`    </v>
+        <v>PLUS_EQUALS,    // Operator `+=`</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3587,7 +3582,7 @@
       </c>
       <c r="E153" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B153,",    // ",C153," `",A153,"`    ",D153)</f>
-        <v>  POWER,    // Operator `^`    </v>
+        <v>POWER,    // Operator `^`</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3603,7 +3598,7 @@
       </c>
       <c r="E154" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B154,",    // ",C154," `",A154,"`    ",D154)</f>
-        <v>  POWER_EQUALS,    // Operator `^=`    </v>
+        <v>POWER_EQUALS,    // Operator `^=`</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3618,7 +3613,7 @@
       </c>
       <c r="E155" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B155,",    // ",C155," `",A155,"`    ",D155)</f>
-        <v>  PROTOCOL,    // Keyword `protocol`    </v>
+        <v>PROTOCOL,    // Keyword `protocol`</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3634,7 +3629,7 @@
       </c>
       <c r="E156" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B156,",    // ",C156," `",A156,"`    ",D156)</f>
-        <v>  QUESTION,    // Punctuation `?`    </v>
+        <v>QUESTION,    // Punctuation `?`</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3652,7 +3647,7 @@
       </c>
       <c r="E157" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B157,",    // ",C157," `",A157,"`    ",D157)</f>
-        <v>  QUESTION_QUESTION,    // Operator `??`    Null coalescence</v>
+        <v>QUESTION_QUESTION,    // Operator `??`    Null coalescence</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3667,7 +3662,7 @@
       </c>
       <c r="E158" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B158,",    // ",C158," `",A158,"`    ",D158)</f>
-        <v>  RAISE,    // Keyword `raise`    </v>
+        <v>RAISE,    // Keyword `raise`</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3686,7 +3681,7 @@
       </c>
       <c r="E159" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B159,",    // ",C159," `",A159,"`    ",D159)</f>
-        <v>  RANGE_EXCLUSIVE,    // Operator `..&lt;`    Range from lower inclusive to upper exclusive</v>
+        <v>RANGE_EXCLUSIVE,    // Operator `..&lt;`    Range from lower inclusive to upper exclusive</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3705,7 +3700,7 @@
       </c>
       <c r="E160" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B160,",    // ",C160," `",A160,"`    ",D160)</f>
-        <v>  RANGE_INCLUSIVE,    // Operator `..`    Range from lower to upper inclusive</v>
+        <v>RANGE_INCLUSIVE,    // Operator `..`    Range from lower to upper inclusive</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3720,7 +3715,7 @@
       </c>
       <c r="E161" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B161,",    // ",C161," `",A161,"`    ",D161)</f>
-        <v>  REGARDLESS,    // Keyword `regardless`    </v>
+        <v>REGARDLESS,    // Keyword `regardless`</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3736,7 +3731,7 @@
       </c>
       <c r="E162" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B162,",    // ",C162," `",A162,"`    ",D162)</f>
-        <v>  RegularExpressionLiteral,    // Literal `~/ ... /igm`    </v>
+        <v>RegularExpressionLiteral,    // Literal `~/ ... /igm`</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3751,7 +3746,7 @@
       </c>
       <c r="E163" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B163,",    // ",C163," `",A163,"`    ",D163)</f>
-        <v>  REPEAT,    // Keyword `repeat`    </v>
+        <v>REPEAT,    // Keyword `repeat`</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3766,7 +3761,7 @@
       </c>
       <c r="E164" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B164,",    // ",C164," `",A164,"`    ",D164)</f>
-        <v>  RETURN,    // Keyword `return`    </v>
+        <v>RETURN,    // Keyword `return`</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3782,7 +3777,7 @@
       </c>
       <c r="E165" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B165,",    // ",C165," `",A165,"`    ",D165)</f>
-        <v>  RIGHT_BRACE,    // Punctuation `}`    </v>
+        <v>RIGHT_BRACE,    // Punctuation `}`</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3798,7 +3793,7 @@
       </c>
       <c r="E166" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B166,",    // ",C166," `",A166,"`    ",D166)</f>
-        <v>  RIGHT_BRACKET,    // Punctuation `]`    </v>
+        <v>RIGHT_BRACKET,    // Punctuation `]`</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3814,7 +3809,7 @@
       </c>
       <c r="E167" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B167,",    // ",C167," `",A167,"`    ",D167)</f>
-        <v>  RIGHT_PARENTHESIS,    // Punctuation `)`    </v>
+        <v>RIGHT_PARENTHESIS,    // Punctuation `)`</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3829,7 +3824,7 @@
       </c>
       <c r="E168" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B168,",    // ",C168," `",A168,"`    ",D168)</f>
-        <v>  RULE,    // Keyword `rule`    </v>
+        <v>RULE,    // Keyword `rule`</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3844,7 +3839,7 @@
       </c>
       <c r="E169" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B169,",    // ",C169," `",A169,"`    ",D169)</f>
-        <v>  SAMPLING,    // Keyword `sampling`    </v>
+        <v>SAMPLING,    // Keyword `sampling`</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3859,7 +3854,7 @@
       </c>
       <c r="E170" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B170,",    // ",C170," `",A170,"`    ",D170)</f>
-        <v>  SCENARIO,    // Keyword `scenario`    </v>
+        <v>SCENARIO,    // Keyword `scenario`</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3874,7 +3869,7 @@
       </c>
       <c r="E171" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B171,",    // ",C171," `",A171,"`    ",D171)</f>
-        <v>  SELECT,    // Keyword `select`    </v>
+        <v>SELECT,    // Keyword `select`</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3889,7 +3884,7 @@
       </c>
       <c r="E172" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B172,",    // ",C172," `",A172,"`    ",D172)</f>
-        <v>  SELF,    // Keyword `self`    </v>
+        <v>SELF,    // Keyword `self`</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3905,7 +3900,7 @@
       </c>
       <c r="E173" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B173,",    // ",C173," `",A173,"`    ",D173)</f>
-        <v>  SEMICOLON,    // Punctuation `;`    </v>
+        <v>SEMICOLON,    // Punctuation `;`</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3920,7 +3915,7 @@
       </c>
       <c r="E174" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B174,",    // ",C174," `",A174,"`    ",D174)</f>
-        <v>  SETUP,    // Keyword `setup`    </v>
+        <v>SETUP,    // Keyword `setup`</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3935,7 +3930,7 @@
       </c>
       <c r="E175" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B175,",    // ",C175," `",A175,"`    ",D175)</f>
-        <v>  SPECIFICATION,    // Keyword `specification`    </v>
+        <v>SPECIFICATION,    // Keyword `specification`</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3950,7 +3945,7 @@
       </c>
       <c r="E176" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B176,",    // ",C176," `",A176,"`    ",D176)</f>
-        <v>  STRUCTURE,    // Keyword `structure`    </v>
+        <v>STRUCTURE,    // Keyword `structure`</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3961,190 +3956,190 @@
         <v>286</v>
       </c>
       <c r="C177" s="0" t="s">
-        <v>7</v>
+        <v>286</v>
       </c>
       <c r="E177" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B177,",    // ",C177," `",A177,"`    ",D177)</f>
-        <v>  SYMBOL,    // Keyword `symbol`    </v>
+        <v>Tag,    // Tag `#abc_def`</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="0" t="s">
+      <c r="A178" s="0" t="str">
+        <f aca="false">"{{{...}}}"</f>
+        <v>{{{...}}}</v>
+      </c>
+      <c r="B178" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="B178" s="0" t="s">
-        <v>288</v>
-      </c>
       <c r="C178" s="0" t="s">
-        <v>288</v>
+        <v>15</v>
       </c>
       <c r="E178" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B178,",    // ",C178," `",A178,"`    ",D178)</f>
-        <v>  Tag,    // Tag `#abc_def`    </v>
+        <v>TemplateLiteral,    // Literal `{{{...}}}`</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="0" t="str">
-        <f aca="false">"{{{...}}}"</f>
-        <v>{{{...}}}</v>
-      </c>
-      <c r="B179" s="3" t="s">
+      <c r="A179" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="B179" s="0" t="s">
         <v>289</v>
       </c>
       <c r="C179" s="0" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E179" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B179,",    // ",C179," `",A179,"`    ",D179)</f>
-        <v>  TemplateLiteral,    // Literal `{{{...}}}`    </v>
+        <v>TEST,    // Keyword `test`</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="0" t="s">
+      <c r="A180" s="0" t="str">
+        <f aca="false">"""..."""</f>
+        <v>"..."</v>
+      </c>
+      <c r="B180" s="0" t="s">
         <v>290</v>
       </c>
-      <c r="B180" s="0" t="s">
-        <v>291</v>
-      </c>
       <c r="C180" s="0" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E180" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B180,",    // ",C180," `",A180,"`    ",D180)</f>
-        <v>  TEST,    // Keyword `test`    </v>
+        <v>TextLiteral_DoubleQuoted,    // Literal `"..."`</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="str">
-        <f aca="false">"""..."""</f>
-        <v>"..."</v>
+        <f aca="false">"""""""..."""""""</f>
+        <v>"""..."""</v>
       </c>
       <c r="B181" s="0" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C181" s="0" t="s">
         <v>15</v>
       </c>
       <c r="E181" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B181,",    // ",C181," `",A181,"`    ",D181)</f>
-        <v>  TextLiteral_DoubleQuoted,    // Literal `"..."`    </v>
+        <v>TextLiteral_DoubleQuotedMultiline,    // Literal `"""..."""`</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="str">
-        <f aca="false">"""""""..."""""""</f>
-        <v>"""..."""</v>
+        <f aca="false">"'...'"</f>
+        <v>'...'</v>
       </c>
       <c r="B182" s="0" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C182" s="0" t="s">
         <v>15</v>
       </c>
       <c r="E182" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B182,",    // ",C182," `",A182,"`    ",D182)</f>
-        <v>  TextLiteral_DoubleQuotedMultiline,    // Literal `"""..."""`    </v>
+        <v>TextLiteral_SingleQuoted,    // Literal `'...'`</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="str">
-        <f aca="false">"'...'"</f>
-        <v>'...'</v>
+        <f aca="false">"'''...'''"</f>
+        <v>'''...'''</v>
       </c>
       <c r="B183" s="0" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C183" s="0" t="s">
         <v>15</v>
       </c>
       <c r="E183" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B183,",    // ",C183," `",A183,"`    ",D183)</f>
-        <v>  TextLiteral_SingleQuoted,    // Literal `'...'`    </v>
+        <v>TextLiteral_SingleQuotedMultiline,    // Literal `'''...'''`</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="0" t="str">
-        <f aca="false">"'''...'''"</f>
-        <v>'''...'''</v>
+      <c r="A184" s="0" t="s">
+        <v>294</v>
       </c>
       <c r="B184" s="0" t="s">
         <v>295</v>
       </c>
       <c r="C184" s="0" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E184" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B184,",    // ",C184," `",A184,"`    ",D184)</f>
-        <v>  TextLiteral_SingleQuotedMultiline,    // Literal `'''...'''`    </v>
+        <v>THEN,    // Keyword `then`</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="0" t="s">
+      <c r="A185" s="0" t="str">
+        <f aca="false">"~"</f>
+        <v>~</v>
+      </c>
+      <c r="B185" s="0" t="s">
         <v>296</v>
       </c>
-      <c r="B185" s="0" t="s">
-        <v>297</v>
-      </c>
       <c r="C185" s="0" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="E185" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B185,",    // ",C185," `",A185,"`    ",D185)</f>
-        <v>  THEN,    // Keyword `then`    </v>
+        <v>TILDE,    // Operator `~`</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="str">
-        <f aca="false">"~"</f>
-        <v>~</v>
+        <f aca="false">"~="</f>
+        <v>~=</v>
       </c>
       <c r="B186" s="0" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C186" s="0" t="s">
         <v>63</v>
       </c>
       <c r="E186" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B186,",    // ",C186," `",A186,"`    ",D186)</f>
-        <v>  TILDE,    // Operator `~`    </v>
+        <v>TILDE_EQUALS,    // Operator `~=`</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="str">
-        <f aca="false">"~="</f>
-        <v>~=</v>
+        <f aca="false">"*"</f>
+        <v>*</v>
       </c>
       <c r="B187" s="0" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C187" s="0" t="s">
         <v>63</v>
       </c>
       <c r="E187" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B187,",    // ",C187," `",A187,"`    ",D187)</f>
-        <v>  TILDE_EQUALS,    // Operator `~=`    </v>
+        <v>TIMES,    // Operator `*`</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="str">
-        <f aca="false">"*"</f>
-        <v>*</v>
+        <f aca="false">"*="</f>
+        <v>*=</v>
       </c>
       <c r="B188" s="0" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C188" s="0" t="s">
         <v>63</v>
       </c>
       <c r="E188" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B188,",    // ",C188," `",A188,"`    ",D188)</f>
-        <v>  TIMES,    // Operator `*`    </v>
+        <v>TIMES_EQUALS,    // Operator `*=`</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A189" s="0" t="str">
-        <f aca="false">"*="</f>
-        <v>*=</v>
+      <c r="A189" s="0" t="s">
+        <v>300</v>
       </c>
       <c r="B189" s="0" t="s">
         <v>301</v>
@@ -4152,27 +4147,27 @@
       <c r="C189" s="0" t="s">
         <v>63</v>
       </c>
+      <c r="D189" s="0" t="s">
+        <v>302</v>
+      </c>
       <c r="E189" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B189,",    // ",C189," `",A189,"`    ",D189)</f>
-        <v>  TIMES_EQUALS,    // Operator `*=`    </v>
+        <v>TO_STRING,    // Operator `$`    Conversion to string (prefix)</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B190" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C190" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="D190" s="0" t="s">
-        <v>304</v>
+        <v>7</v>
       </c>
       <c r="E190" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B190,",    // ",C190," `",A190,"`    ",D190)</f>
-        <v>  TO_STRING,    // Operator `$`    Conversion to string (prefix)</v>
+        <v>TRANSFORM,    // Keyword `transform`</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4187,14 +4182,14 @@
       </c>
       <c r="E191" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B191,",    // ",C191," `",A191,"`    ",D191)</f>
-        <v>  TRANSFORM,    // Keyword `transform`    </v>
+        <v>TRANSLATE,    // Keyword `translate`</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A192" s="0" t="s">
+      <c r="A192" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="B192" s="0" t="s">
+      <c r="B192" s="2" t="s">
         <v>308</v>
       </c>
       <c r="C192" s="0" t="s">
@@ -4202,14 +4197,14 @@
       </c>
       <c r="E192" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B192,",    // ",C192," `",A192,"`    ",D192)</f>
-        <v>  TRANSLATE,    // Keyword `translate`    </v>
+        <v>TRUE,    // Keyword `true`</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="2" t="s">
+      <c r="A193" s="0" t="s">
         <v>309</v>
       </c>
-      <c r="B193" s="2" t="s">
+      <c r="B193" s="0" t="s">
         <v>310</v>
       </c>
       <c r="C193" s="0" t="s">
@@ -4217,7 +4212,7 @@
       </c>
       <c r="E193" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B193,",    // ",C193," `",A193,"`    ",D193)</f>
-        <v>  TRUE,    // Keyword `true`    </v>
+        <v>TYPE,    // Keyword `type`</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4232,7 +4227,7 @@
       </c>
       <c r="E194" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B194,",    // ",C194," `",A194,"`    ",D194)</f>
-        <v>  TYPE,    // Keyword `type`    </v>
+        <v>UNDEFINED,    // Keyword `undefined`</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4247,7 +4242,7 @@
       </c>
       <c r="E195" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B195,",    // ",C195," `",A195,"`    ",D195)</f>
-        <v>  UNDEFINED,    // Keyword `undefined`    </v>
+        <v>UNION,    // Keyword `union`</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4262,7 +4257,7 @@
       </c>
       <c r="E196" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B196,",    // ",C196," `",A196,"`    ",D196)</f>
-        <v>  UNION,    // Keyword `union`    </v>
+        <v>UNLESS,    // Keyword `unless`</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4277,7 +4272,7 @@
       </c>
       <c r="E197" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B197,",    // ",C197," `",A197,"`    ",D197)</f>
-        <v>  UNLESS,    // Keyword `unless`    </v>
+        <v>UNTIL,    // Keyword `until`</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4292,7 +4287,7 @@
       </c>
       <c r="E198" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B198,",    // ",C198," `",A198,"`    ",D198)</f>
-        <v>  UNTIL,    // Keyword `until`    </v>
+        <v>UPDATE,    // Keyword `update`</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4307,28 +4302,32 @@
       </c>
       <c r="E199" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B199,",    // ",C199," `",A199,"`    ",D199)</f>
-        <v>  UPDATE,    // Keyword `update`    </v>
+        <v>USE,    // Keyword `use`</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A200" s="0" t="s">
+      <c r="A200" s="0" t="str">
+        <f aca="false">"#{...}"</f>
+        <v>#{...}</v>
+      </c>
+      <c r="B200" s="0" t="s">
         <v>323</v>
       </c>
-      <c r="B200" s="0" t="s">
+      <c r="C200" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D200" s="0" t="s">
         <v>324</v>
-      </c>
-      <c r="C200" s="0" t="s">
-        <v>7</v>
       </c>
       <c r="E200" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B200,",    // ",C200," `",A200,"`    ",D200)</f>
-        <v>  USE,    // Keyword `use`    </v>
+        <v>UserDefinedLiteral_Braces,    // Literal `#{...}`    User-defined literal B</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="str">
-        <f aca="false">"#{...}"</f>
-        <v>#{...}</v>
+        <f aca="false">"#[...]"</f>
+        <v>#[...]</v>
       </c>
       <c r="B201" s="0" t="s">
         <v>325</v>
@@ -4341,13 +4340,13 @@
       </c>
       <c r="E201" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B201,",    // ",C201," `",A201,"`    ",D201)</f>
-        <v>  UserDefinedLiteral_Braces,    // Literal `#{...}`    User-defined literal B</v>
+        <v>UserDefinedLiteral_Brackets,    // Literal `#[...]`    User-defined literal A</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="str">
-        <f aca="false">"#[...]"</f>
-        <v>#[...]</v>
+        <f aca="false">"#/.../"</f>
+        <v>#/.../</v>
       </c>
       <c r="B202" s="0" t="s">
         <v>327</v>
@@ -4360,26 +4359,22 @@
       </c>
       <c r="E202" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B202,",    // ",C202," `",A202,"`    ",D202)</f>
-        <v>  UserDefinedLiteral_Brackets,    // Literal `#[...]`    User-defined literal A</v>
+        <v>UserDefinedLiteral_Slashes,    // Literal `#/.../`    User-defined literal C</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="0" t="str">
-        <f aca="false">"#/.../"</f>
-        <v>#/.../</v>
+      <c r="A203" s="0" t="s">
+        <v>329</v>
       </c>
       <c r="B203" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C203" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D203" s="0" t="s">
-        <v>330</v>
+        <v>7</v>
       </c>
       <c r="E203" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B203,",    // ",C203," `",A203,"`    ",D203)</f>
-        <v>  UserDefinedLiteral_Slashes,    // Literal `#/.../`    User-defined literal C</v>
+        <v>VALUE,    // Keyword `value`</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4394,7 +4389,7 @@
       </c>
       <c r="E204" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B204,",    // ",C204," `",A204,"`    ",D204)</f>
-        <v>  VALUE,    // Keyword `value`    </v>
+        <v>VARIABLE,    // Keyword `variable`</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4409,7 +4404,7 @@
       </c>
       <c r="E205" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B205,",    // ",C205," `",A205,"`    ",D205)</f>
-        <v>  VARIABLE,    // Keyword `variable`    </v>
+        <v>VARIANT,    // Keyword `variant`</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4424,38 +4419,38 @@
       </c>
       <c r="E206" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B206,",    // ",C206," `",A206,"`    ",D206)</f>
-        <v>  VARIANT,    // Keyword `variant`    </v>
+        <v>VERSION,    // Keyword `version`</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A207" s="0" t="s">
+      <c r="A207" s="0" t="str">
+        <f aca="false">"2.3.4"</f>
+        <v>2.3.4</v>
+      </c>
+      <c r="B207" s="0" t="s">
         <v>337</v>
       </c>
-      <c r="B207" s="0" t="s">
-        <v>338</v>
-      </c>
       <c r="C207" s="0" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E207" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B207,",    // ",C207," `",A207,"`    ",D207)</f>
-        <v>  VERSION,    // Keyword `version`    </v>
+        <v>VersionLiteral,    // Literal `2.3.4`</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A208" s="0" t="str">
-        <f aca="false">"2.3.4"</f>
-        <v>2.3.4</v>
+      <c r="A208" s="0" t="s">
+        <v>338</v>
       </c>
       <c r="B208" s="0" t="s">
         <v>339</v>
       </c>
       <c r="C208" s="0" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E208" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B208,",    // ",C208," `",A208,"`    ",D208)</f>
-        <v>  VersionLiteral,    // Literal `2.3.4`    </v>
+        <v>VERTEX,    // Keyword `vertex`</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4470,7 +4465,7 @@
       </c>
       <c r="E209" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B209,",    // ",C209," `",A209,"`    ",D209)</f>
-        <v>  VERTEX,    // Keyword `vertex`    </v>
+        <v>WHEN,    // Keyword `when`</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4485,7 +4480,7 @@
       </c>
       <c r="E210" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B210,",    // ",C210," `",A210,"`    ",D210)</f>
-        <v>  WHEN,    // Keyword `when`    </v>
+        <v>WHERE,    // Keyword `where`</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4500,7 +4495,7 @@
       </c>
       <c r="E211" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B211,",    // ",C211," `",A211,"`    ",D211)</f>
-        <v>  WHERE,    // Keyword `where`    </v>
+        <v>WHILE,    // Keyword `while`</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4515,7 +4510,7 @@
       </c>
       <c r="E212" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B212,",    // ",C212," `",A212,"`    ",D212)</f>
-        <v>  WHILE,    // Keyword `while`    </v>
+        <v>WITH,    // Keyword `with`</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4530,7 +4525,7 @@
       </c>
       <c r="E213" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B213,",    // ",C213," `",A213,"`    ",D213)</f>
-        <v>  WITH,    // Keyword `with`    </v>
+        <v>XOR,    // Keyword `xor`</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4545,22 +4540,7 @@
       </c>
       <c r="E214" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B214,",    // ",C214," `",A214,"`    ",D214)</f>
-        <v>  XOR,    // Keyword `xor`    </v>
-      </c>
-    </row>
-    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A215" s="0" t="s">
-        <v>352</v>
-      </c>
-      <c r="B215" s="0" t="s">
-        <v>353</v>
-      </c>
-      <c r="C215" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E215" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B215,",    // ",C215," `",A215,"`    ",D215)</f>
-        <v>  YIELD,    // Keyword `yield`    </v>
+        <v>YIELD,    // Keyword `yield`</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added function expression literals.
</commit_message>
<xml_diff>
--- a/barlom-language/lexer/doc/TokenTypes.xlsx
+++ b/barlom-language/lexer/doc/TokenTypes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="204">
   <si>
     <t>Token Text</t>
   </si>
@@ -176,6 +176,12 @@
   </si>
   <si>
     <t>Operator</t>
+  </si>
+  <si>
+    <t>begin</t>
+  </si>
+  <si>
+    <t>BEGIN</t>
   </si>
   <si>
     <t>~and~</t>
@@ -748,20 +754,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E139"/>
+  <dimension ref="A1:E140"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E42" activeCellId="0" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.7704081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.0765306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="73.030612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.234693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="72.2193877551021"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -793,7 +799,7 @@
       </c>
       <c r="E2" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B2,",    // ",C2," `",A2,"`    ",D2)</f>
-        <v>  AND,    // Keyword `and`    </v>
+        <v>AND,    // Keyword `and`</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -809,7 +815,7 @@
       </c>
       <c r="E3" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B3,",    // ",C3," `",A3,"`    ",D3)</f>
-        <v>  ANONYMOUS_LITERAL,    // Literal `_`    </v>
+        <v>ANONYMOUS_LITERAL,    // Literal `_`</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -825,7 +831,7 @@
       </c>
       <c r="E4" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B4,",    // ",C4," `",A4,"`    ",D4)</f>
-        <v>  ARROW_COLON_COLON_LEFT,    // Arrow `&lt;::`    </v>
+        <v>ARROW_COLON_COLON_LEFT,    // Arrow `&lt;::`</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -841,7 +847,7 @@
       </c>
       <c r="E5" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B5,",    // ",C5," `",A5,"`    ",D5)</f>
-        <v>  ARROW_COLON_COLON_LEFT_RIGHT,    // Arrow `&lt;::&gt;`    </v>
+        <v>ARROW_COLON_COLON_LEFT_RIGHT,    // Arrow `&lt;::&gt;`</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -857,7 +863,7 @@
       </c>
       <c r="E6" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B6,",    // ",C6," `",A6,"`    ",D6)</f>
-        <v>  ARROW_COLON_COLON_RIGHT,    // Arrow `::&gt;`    </v>
+        <v>ARROW_COLON_COLON_RIGHT,    // Arrow `::&gt;`</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -873,7 +879,7 @@
       </c>
       <c r="E7" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B7,",    // ",C7," `",A7,"`    ",D7)</f>
-        <v>  ARROW_COLON_LEFT,    // Arrow `&lt;:`    </v>
+        <v>ARROW_COLON_LEFT,    // Arrow `&lt;:`</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -889,7 +895,7 @@
       </c>
       <c r="E8" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B8,",    // ",C8," `",A8,"`    ",D8)</f>
-        <v>  ARROW_COLON_LEFT_RIGHT,    // Arrow `&lt;:&gt;`    </v>
+        <v>ARROW_COLON_LEFT_RIGHT,    // Arrow `&lt;:&gt;`</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -905,7 +911,7 @@
       </c>
       <c r="E9" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B9,",    // ",C9," `",A9,"`    ",D9)</f>
-        <v>  ARROW_COLON_RIGHT,    // Arrow `:&gt;`    </v>
+        <v>ARROW_COLON_RIGHT,    // Arrow `:&gt;`</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -921,7 +927,7 @@
       </c>
       <c r="E10" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B10,",    // ",C10," `",A10,"`    ",D10)</f>
-        <v>  ARROW_DASH_DASH_DASH,    // Arrow `---`    </v>
+        <v>ARROW_DASH_DASH_DASH,    // Arrow `---`</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -937,7 +943,7 @@
       </c>
       <c r="E11" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B11,",    // ",C11," `",A11,"`    ",D11)</f>
-        <v>  ARROW_DASH_DASH_DIAMOND_LEFT,    // Arrow `&lt;&gt;--`    </v>
+        <v>ARROW_DASH_DASH_DIAMOND_LEFT,    // Arrow `&lt;&gt;--`</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -953,7 +959,7 @@
       </c>
       <c r="E12" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B12,",    // ",C12," `",A12,"`    ",D12)</f>
-        <v>  ARROW_DASH_DASH_DIAMOND_RIGHT,    // Arrow `--&lt;&gt;`    </v>
+        <v>ARROW_DASH_DASH_DIAMOND_RIGHT,    // Arrow `--&lt;&gt;`</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -969,7 +975,7 @@
       </c>
       <c r="E13" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B13,",    // ",C13," `",A13,"`    ",D13)</f>
-        <v>  ARROW_DASH_DASH_DOUBLE_LEFT,    // Arrow `&lt;&lt;--`    </v>
+        <v>ARROW_DASH_DASH_DOUBLE_LEFT,    // Arrow `&lt;&lt;--`</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -985,7 +991,7 @@
       </c>
       <c r="E14" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B14,",    // ",C14," `",A14,"`    ",D14)</f>
-        <v>  ARROW_DASH_DASH_DOUBLE_RIGHT,    // Arrow `--&gt;&gt;`    </v>
+        <v>ARROW_DASH_DASH_DOUBLE_RIGHT,    // Arrow `--&gt;&gt;`</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1001,7 +1007,7 @@
       </c>
       <c r="E15" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B15,",    // ",C15," `",A15,"`    ",D15)</f>
-        <v>  ARROW_DASH_DASH_LEFT,    // Arrow `&lt;--`    </v>
+        <v>ARROW_DASH_DASH_LEFT,    // Arrow `&lt;--`</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1017,7 +1023,7 @@
       </c>
       <c r="E16" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B16,",    // ",C16," `",A16,"`    ",D16)</f>
-        <v>  ARROW_DASH_DASH_LEFT_RIGHT,    // Arrow `&lt;--&gt;`    </v>
+        <v>ARROW_DASH_DASH_LEFT_RIGHT,    // Arrow `&lt;--&gt;`</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1033,7 +1039,7 @@
       </c>
       <c r="E17" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B17,",    // ",C17," `",A17,"`    ",D17)</f>
-        <v>  ARROW_DASH_DASH_RIGHT,    // Arrow `--&gt;`    </v>
+        <v>ARROW_DASH_DASH_RIGHT,    // Arrow `--&gt;`</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1049,7 +1055,7 @@
       </c>
       <c r="E18" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B18,",    // ",C18," `",A18,"`    ",D18)</f>
-        <v>  ARROW_DASH_LEFT,    // Arrow `&lt;-`    </v>
+        <v>ARROW_DASH_LEFT,    // Arrow `&lt;-`</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1065,7 +1071,7 @@
       </c>
       <c r="E19" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B19,",    // ",C19," `",A19,"`    ",D19)</f>
-        <v>  ARROW_DASH_LEFT_RIGHT,    // Arrow `&lt;-&gt;`    </v>
+        <v>ARROW_DASH_LEFT_RIGHT,    // Arrow `&lt;-&gt;`</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1081,7 +1087,7 @@
       </c>
       <c r="E20" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B20,",    // ",C20," `",A20,"`    ",D20)</f>
-        <v>  ARROW_DASH_RIGHT,    // Arrow `-&gt;`    </v>
+        <v>ARROW_DASH_RIGHT,    // Arrow `-&gt;`</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1097,7 +1103,7 @@
       </c>
       <c r="E21" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B21,",    // ",C21," `",A21,"`    ",D21)</f>
-        <v>  ARROW_EQUAL_EQUAL_DIAMOND_LEFT,    // Arrow `&lt;&gt;==`    </v>
+        <v>ARROW_EQUAL_EQUAL_DIAMOND_LEFT,    // Arrow `&lt;&gt;==`</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1113,7 +1119,7 @@
       </c>
       <c r="E22" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B22,",    // ",C22," `",A22,"`    ",D22)</f>
-        <v>  ARROW_EQUAL_EQUAL_DIAMOND_RIGHT,    // Arrow `==&lt;&gt;`    </v>
+        <v>ARROW_EQUAL_EQUAL_DIAMOND_RIGHT,    // Arrow `==&lt;&gt;`</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1129,7 +1135,7 @@
       </c>
       <c r="E23" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B23,",    // ",C23," `",A23,"`    ",D23)</f>
-        <v>  ARROW_EQUAL_EQUAL_DOUBLE_LEFT,    // Arrow `&lt;&lt;==`    </v>
+        <v>ARROW_EQUAL_EQUAL_DOUBLE_LEFT,    // Arrow `&lt;&lt;==`</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1145,7 +1151,7 @@
       </c>
       <c r="E24" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B24,",    // ",C24," `",A24,"`    ",D24)</f>
-        <v>  ARROW_EQUAL_EQUAL_DOUBLE_RIGHT,    // Arrow `==&gt;&gt;`    </v>
+        <v>ARROW_EQUAL_EQUAL_DOUBLE_RIGHT,    // Arrow `==&gt;&gt;`</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1161,7 +1167,7 @@
       </c>
       <c r="E25" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B25,",    // ",C25," `",A25,"`    ",D25)</f>
-        <v>  ARROW_EQUAL_EQUAL_LEFT,    // Arrow `&lt;==`    </v>
+        <v>ARROW_EQUAL_EQUAL_LEFT,    // Arrow `&lt;==`</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1177,7 +1183,7 @@
       </c>
       <c r="E26" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B26,",    // ",C26," `",A26,"`    ",D26)</f>
-        <v>  ARROW_EQUAL_EQUAL_LEFT_RIGHT,    // Arrow `&lt;==&gt;`    </v>
+        <v>ARROW_EQUAL_EQUAL_LEFT_RIGHT,    // Arrow `&lt;==&gt;`</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1193,7 +1199,7 @@
       </c>
       <c r="E27" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B27,",    // ",C27," `",A27,"`    ",D27)</f>
-        <v>  ARROW_EQUAL_EQUAL_RIGHT,    // Arrow `==&gt;`    </v>
+        <v>ARROW_EQUAL_EQUAL_RIGHT,    // Arrow `==&gt;`</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1209,7 +1215,7 @@
       </c>
       <c r="E28" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B28,",    // ",C28," `",A28,"`    ",D28)</f>
-        <v>  ARROW_EQUAL_RIGHT,    // Arrow `=&gt;`    </v>
+        <v>ARROW_EQUAL_RIGHT,    // Arrow `=&gt;`</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1225,7 +1231,7 @@
       </c>
       <c r="E29" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B29,",    // ",C29," `",A29,"`    ",D29)</f>
-        <v>  ARROW_TILDE_LEFT,    // Arrow `&lt;~`    </v>
+        <v>ARROW_TILDE_LEFT,    // Arrow `&lt;~`</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1241,7 +1247,7 @@
       </c>
       <c r="E30" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B30,",    // ",C30," `",A30,"`    ",D30)</f>
-        <v>  ARROW_TILDE_LEFT_RIGHT,    // Arrow `&lt;~&gt;`    </v>
+        <v>ARROW_TILDE_LEFT_RIGHT,    // Arrow `&lt;~&gt;`</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1257,7 +1263,7 @@
       </c>
       <c r="E31" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B31,",    // ",C31," `",A31,"`    ",D31)</f>
-        <v>  ARROW_TILDE_RIGHT,    // Arrow `~&gt;`    </v>
+        <v>ARROW_TILDE_RIGHT,    // Arrow `~&gt;`</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1273,7 +1279,7 @@
       </c>
       <c r="E32" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B32,",    // ",C32," `",A32,"`    ",D32)</f>
-        <v>  ARROW_TILDE_TILDE_DIAMOND_LEFT,    // Arrow `&lt;&gt;~~`    </v>
+        <v>ARROW_TILDE_TILDE_DIAMOND_LEFT,    // Arrow `&lt;&gt;~~`</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1289,7 +1295,7 @@
       </c>
       <c r="E33" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B33,",    // ",C33," `",A33,"`    ",D33)</f>
-        <v>  ARROW_TILDE_TILDE_DIAMOND_RIGHT,    // Arrow `~~&lt;&gt;`    </v>
+        <v>ARROW_TILDE_TILDE_DIAMOND_RIGHT,    // Arrow `~~&lt;&gt;`</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1305,7 +1311,7 @@
       </c>
       <c r="E34" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B34,",    // ",C34," `",A34,"`    ",D34)</f>
-        <v>  ARROW_TILDE_TILDE_DOUBLE_LEFT,    // Arrow `&lt;&lt;~~`    </v>
+        <v>ARROW_TILDE_TILDE_DOUBLE_LEFT,    // Arrow `&lt;&lt;~~`</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1321,7 +1327,7 @@
       </c>
       <c r="E35" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B35,",    // ",C35," `",A35,"`    ",D35)</f>
-        <v>  ARROW_TILDE_TILDE_DOUBLE_RIGHT,    // Arrow `~~&gt;&gt;`    </v>
+        <v>ARROW_TILDE_TILDE_DOUBLE_RIGHT,    // Arrow `~~&gt;&gt;`</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1337,7 +1343,7 @@
       </c>
       <c r="E36" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B36,",    // ",C36," `",A36,"`    ",D36)</f>
-        <v>  ARROW_TILDE_TILDE_LEFT,    // Arrow `&lt;~~`    </v>
+        <v>ARROW_TILDE_TILDE_LEFT,    // Arrow `&lt;~~`</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1353,7 +1359,7 @@
       </c>
       <c r="E37" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B37,",    // ",C37," `",A37,"`    ",D37)</f>
-        <v>  ARROW_TILDE_TILDE_LEFT_RIGHT,    // Arrow `&lt;~~&gt;`    </v>
+        <v>ARROW_TILDE_TILDE_LEFT_RIGHT,    // Arrow `&lt;~~&gt;`</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1369,7 +1375,7 @@
       </c>
       <c r="E38" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B38,",    // ",C38," `",A38,"`    ",D38)</f>
-        <v>  ARROW_TILDE_TILDE_RIGHT,    // Arrow `~~&gt;`    </v>
+        <v>ARROW_TILDE_TILDE_RIGHT,    // Arrow `~~&gt;`</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1385,7 +1391,7 @@
       </c>
       <c r="E39" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B39,",    // ",C39," `",A39,"`    ",D39)</f>
-        <v>  ARROW_TILDE_TILDE_TILDE,    // Arrow `~~~`    </v>
+        <v>ARROW_TILDE_TILDE_TILDE,    // Arrow `~~~`</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1400,7 +1406,7 @@
       </c>
       <c r="E40" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B40,",    // ",C40," `",A40,"`    ",D40)</f>
-        <v>  AS,    // Keyword `as`    </v>
+        <v>AS,    // Keyword `as`</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1415,7 +1421,7 @@
       </c>
       <c r="E41" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B41,",    // ",C41," `",A41,"`    ",D41)</f>
-        <v>  AT,    // Operator `@`    </v>
+        <v>AT,    // Operator `@`</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1426,399 +1432,399 @@
         <v>53</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D42" s="0" t="s">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="E42" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B42,",    // ",C42," `",A42,"`    ",D42)</f>
-        <v>  BITWISE_AND,    // Operator `~and~`    Bitwise AND</v>
+        <v>  BEGIN,    // Keyword `begin`    </v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B43" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="B43" s="0" t="s">
+      <c r="C43" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D43" s="0" t="s">
         <v>56</v>
-      </c>
-      <c r="C43" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D43" s="0" t="s">
-        <v>57</v>
       </c>
       <c r="E43" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B43,",    // ",C43," `",A43,"`    ",D43)</f>
-        <v>  BITWISE_NAND,    // Operator `~nand~`    Bitwise NAND</v>
+        <v>BITWISE_AND,    // Operator `~and~`    Bitwise AND</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B44" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="B44" s="0" t="s">
+      <c r="C44" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D44" s="0" t="s">
         <v>59</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D44" s="0" t="s">
-        <v>60</v>
       </c>
       <c r="E44" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B44,",    // ",C44," `",A44,"`    ",D44)</f>
-        <v>  BITWISE_NOR,    // Operator `~nor~`    Bitwise NOR</v>
+        <v>BITWISE_NAND,    // Operator `~nand~`    Bitwise NAND</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B45" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="B45" s="0" t="s">
+      <c r="C45" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D45" s="0" t="s">
         <v>62</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D45" s="0" t="s">
-        <v>63</v>
       </c>
       <c r="E45" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B45,",    // ",C45," `",A45,"`    ",D45)</f>
-        <v>  BITWISE_NOT,    // Operator `~not~`    Bitwise NOT (prefix)</v>
+        <v>BITWISE_NOR,    // Operator `~nor~`    Bitwise NOR</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B46" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="B46" s="0" t="s">
+      <c r="C46" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D46" s="0" t="s">
         <v>65</v>
-      </c>
-      <c r="C46" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D46" s="0" t="s">
-        <v>66</v>
       </c>
       <c r="E46" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B46,",    // ",C46," `",A46,"`    ",D46)</f>
-        <v>  BITWISE_OR,    // Operator `~or~`    Bitwise OR</v>
+        <v>BITWISE_NOT,    // Operator `~not~`    Bitwise NOT (prefix)</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B47" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="B47" s="0" t="s">
+      <c r="C47" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D47" s="0" t="s">
         <v>68</v>
-      </c>
-      <c r="C47" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D47" s="0" t="s">
-        <v>69</v>
       </c>
       <c r="E47" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B47,",    // ",C47," `",A47,"`    ",D47)</f>
-        <v>  BITWISE_SHIFT_LEFT,    // Operator `~shl~`    Bitwise SHIFT LEFT</v>
+        <v>BITWISE_OR,    // Operator `~or~`    Bitwise OR</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B48" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="B48" s="0" t="s">
+      <c r="C48" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D48" s="0" t="s">
         <v>71</v>
-      </c>
-      <c r="C48" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D48" s="0" t="s">
-        <v>72</v>
       </c>
       <c r="E48" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B48,",    // ",C48," `",A48,"`    ",D48)</f>
-        <v>  BITWISE_SHIFT_RIGHT,    // Operator `~shr~`    Bitwise SHIFT RIGHT (sign extend)</v>
+        <v>BITWISE_SHIFT_LEFT,    // Operator `~shl~`    Bitwise SHIFT LEFT</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B49" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="B49" s="0" t="s">
+      <c r="C49" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D49" s="0" t="s">
         <v>74</v>
-      </c>
-      <c r="C49" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D49" s="0" t="s">
-        <v>75</v>
       </c>
       <c r="E49" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B49,",    // ",C49," `",A49,"`    ",D49)</f>
-        <v>  BITWISE_XOR,    // Operator `~xor~`    Bitwise XOR</v>
+        <v>BITWISE_SHIFT_RIGHT,    // Operator `~shr~`    Bitwise SHIFT RIGHT (sign extend)</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B50" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="B50" s="0" t="s">
+      <c r="C50" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D50" s="0" t="s">
         <v>77</v>
-      </c>
-      <c r="C50" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D50" s="0" t="s">
-        <v>78</v>
       </c>
       <c r="E50" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B50,",    // ",C50," `",A50,"`    ",D50)</f>
-        <v>  BITWISE_ZERO_SHIFT_RIGHT,    // Operator `~zshr~`    Bitwise SHIFT RIGHT (zero extend)</v>
+        <v>BITWISE_XOR,    // Operator `~xor~`    Bitwise XOR</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="str">
+      <c r="A51" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="E51" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B51,",    // ",C51," `",A51,"`    ",D51)</f>
+        <v>BITWISE_ZERO_SHIFT_RIGHT,    // Operator `~zshr~`    Bitwise SHIFT RIGHT (zero extend)</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="str">
         <f aca="false">"`...`"</f>
         <v>`...`</v>
       </c>
-      <c r="B51" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="C51" s="0" t="s">
+      <c r="B52" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C52" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="E51" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B51,",    // ",C51," `",A51,"`    ",D51)</f>
-        <v>  CodeLiteral,    // Literal ``...``    </v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="str">
+      <c r="E52" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B52,",    // ",C52," `",A52,"`    ",D52)</f>
+        <v>CodeLiteral,    // Literal ``...``</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="str">
         <f aca="false">":"</f>
         <v>:</v>
       </c>
-      <c r="B52" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="C52" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="E52" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B52,",    // ",C52," `",A52,"`    ",D52)</f>
-        <v>  COLON,    // Punctuation `:`    </v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="str">
+      <c r="B53" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="E53" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B53,",    // ",C53," `",A53,"`    ",D53)</f>
+        <v>COLON,    // Punctuation `:`</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="str">
         <f aca="false">"::"</f>
         <v>::</v>
       </c>
-      <c r="B53" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="C53" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="E53" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B53,",    // ",C53," `",A53,"`    ",D53)</f>
-        <v>  COLON_COLON,    // Punctuation `::`    </v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="str">
+      <c r="B54" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="E54" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B54,",    // ",C54," `",A54,"`    ",D54)</f>
+        <v>COLON_COLON,    // Punctuation `::`</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="str">
         <f aca="false">","</f>
         <v>,</v>
       </c>
-      <c r="B54" s="0" t="s">
+      <c r="B55" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="C55" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="C54" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="E54" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B54,",    // ",C54," `",A54,"`    ",D54)</f>
-        <v>  COMMA,    // Punctuation `,`    </v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="str">
+      <c r="E55" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B55,",    // ",C55," `",A55,"`    ",D55)</f>
+        <v>COMMA,    // Punctuation `,`</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="str">
         <f aca="false">"&lt;=&gt;"</f>
         <v>&lt;=&gt;</v>
       </c>
-      <c r="B55" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="C55" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="E55" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B55,",    // ",C55," `",A55,"`    ",D55)</f>
-        <v>  COMPARE,    // Operator `&lt;=&gt;`    </v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="str">
+      <c r="B56" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E56" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B56,",    // ",C56," `",A56,"`    ",D56)</f>
+        <v>COMPARE,    // Operator `&lt;=&gt;`</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="str">
         <f aca="false">"&amp;="</f>
         <v>&amp;=</v>
       </c>
-      <c r="B56" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="C56" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="E56" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B56,",    // ",C56," `",A56,"`    ",D56)</f>
-        <v>  CONCAT_EQUALS,    // Operator `&amp;=`    </v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="str">
+      <c r="B57" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E57" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B57,",    // ",C57," `",A57,"`    ",D57)</f>
+        <v>CONCAT_EQUALS,    // Operator `&amp;=`</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="str">
         <f aca="false">"&amp;"</f>
         <v>&amp;</v>
       </c>
-      <c r="B57" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="C57" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="E57" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B57,",    // ",C57," `",A57,"`    ",D57)</f>
-        <v>  CONCATENATE,    // Operator `&amp;`    </v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="str">
+      <c r="B58" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E58" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B58,",    // ",C58," `",A58,"`    ",D58)</f>
+        <v>CONCATENATE,    // Operator `&amp;`</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="str">
         <f aca="false">"$2016-12-31T12:01:14.001-05:00$"</f>
         <v>$2016-12-31T12:01:14.001-05:00$</v>
       </c>
-      <c r="B58" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="C58" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E58" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B58,",    // ",C58," `",A58,"`    ",D58)</f>
-        <v>  DateTimeLiteral,    // Literal `$2016-12-31T12:01:14.001-05:00$`    </v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
-        <v>88</v>
-      </c>
       <c r="B59" s="0" t="s">
         <v>89</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E59" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B59,",    // ",C59," `",A59,"`    ",D59)</f>
-        <v>  DIV,    // Keyword `div`    </v>
+        <v>DateTimeLiteral,    // Literal `$2016-12-31T12:01:14.001-05:00$`</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="str">
+      <c r="A60" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E60" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B60,",    // ",C60," `",A60,"`    ",D60)</f>
+        <v>DIV,    // Keyword `div`</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="str">
         <f aca="false">"/="</f>
         <v>/=</v>
       </c>
-      <c r="B60" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="C60" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="E60" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B60,",    // ",C60," `",A60,"`    ",D60)</f>
-        <v>  DIVIDE_EQUALS,    // Operator `/=`    </v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="str">
+      <c r="B61" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E61" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B61,",    // ",C61," `",A61,"`    ",D61)</f>
+        <v>DIVIDE_EQUALS,    // Operator `/=`</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="str">
         <f aca="false">"/"</f>
         <v>/</v>
       </c>
-      <c r="B61" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="C61" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="E61" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B61,",    // ",C61," `",A61,"`    ",D61)</f>
-        <v>  DIVIDED_BY,    // Operator `/`    </v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="str">
+      <c r="B62" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E62" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B62,",    // ",C62," `",A62,"`    ",D62)</f>
+        <v>DIVIDED_BY,    // Operator `/`</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="str">
         <f aca="false">"/*...*/"</f>
         <v>/*...*/</v>
       </c>
-      <c r="B62" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="C62" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="D62" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="E62" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B62,",    // ",C62," `",A62,"`    ",D62)</f>
-        <v>  Documentation,    // Documentation `/*...*/`    Annotation documentation for an element</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="str">
+      <c r="B63" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="E63" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B63,",    // ",C63," `",A63,"`    ",D63)</f>
+        <v>Documentation,    // Documentation `/*...*/`    Annotation documentation for an element</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="str">
         <f aca="false">"."</f>
         <v>.</v>
       </c>
-      <c r="B63" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="C63" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="E63" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B63,",    // ",C63," `",A63,"`    ",D63)</f>
-        <v>  DOT,    // Punctuation `.`    </v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="str">
+      <c r="B64" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="E64" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B64,",    // ",C64," `",A64,"`    ",D64)</f>
+        <v>DOT,    // Punctuation `.`</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="str">
         <f aca="false">"..."</f>
         <v>...</v>
       </c>
-      <c r="B64" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="C64" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="E64" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B64,",    // ",C64," `",A64,"`    ",D64)</f>
-        <v>  DOT_DOT_DOT,    // Punctuation `...`    </v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
-        <v>96</v>
-      </c>
       <c r="B65" s="0" t="s">
         <v>97</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E65" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B65,",    // ",C65," `",A65,"`    ",D65)</f>
-        <v>  DOT_QUESTION,    // Punctuation `.?`    </v>
+        <v>DOT_DOT_DOT,    // Punctuation `...`</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1829,39 +1835,42 @@
         <v>99</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>7</v>
+        <v>83</v>
       </c>
       <c r="E66" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B66,",    // ",C66," `",A66,"`    ",D66)</f>
-        <v>  END,    // Keyword `end`    </v>
+        <v>DOT_QUESTION,    // Punctuation `.?`</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="str">
+      <c r="A67" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E67" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B67,",    // ",C67," `",A67,"`    ",D67)</f>
+        <v>END,    // Keyword `end`</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="str">
         <f aca="false">"="</f>
         <v>=</v>
       </c>
-      <c r="B67" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="C67" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="E67" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B67,",    // ",C67," `",A67,"`    ",D67)</f>
-        <v>  EQUALS,    // Operator `=`    </v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>102</v>
+        <v>51</v>
       </c>
       <c r="E68" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B68,",    // ",C68," `",A68,"`    ",D68)</f>
-        <v>  ErrorInvalidIdentifier,    // Error ``    </v>
+        <v>EQUALS,    // Operator `=`</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1869,309 +1878,306 @@
         <v>103</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E69" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B69,",    // ",C69," `",A69,"`    ",D69)</f>
-        <v>  ErrorInvalidMultilineTextLiteral,    // Error ``    </v>
+        <v>ErrorInvalidIdentifier,    // Error ``</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="C70" s="0" t="s">
         <v>104</v>
-      </c>
-      <c r="C70" s="0" t="s">
-        <v>102</v>
       </c>
       <c r="E70" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B70,",    // ",C70," `",A70,"`    ",D70)</f>
-        <v>  ErrorInvalidTextLiteral,    // Error ``    </v>
+        <v>ErrorInvalidMultilineTextLiteral,    // Error ``</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E71" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B71,",    // ",C71," `",A71,"`    ",D71)</f>
-        <v>  ErrorInvalidTimeLiteral,    // Error ``    </v>
+        <v>ErrorInvalidTextLiteral,    // Error ``</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E72" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B72,",    // ",C72," `",A72,"`    ",D72)</f>
-        <v>  ErrorUnclosedBlockComment,    // Error ``    </v>
+        <v>ErrorInvalidTimeLiteral,    // Error ``</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E73" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B73,",    // ",C73," `",A73,"`    ",D73)</f>
-        <v>  ErrorUnclosedCodeLiteral,    // Error ``    </v>
+        <v>ErrorUnclosedBlockComment,    // Error ``</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E74" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B74,",    // ",C74," `",A74,"`    ",D74)</f>
-        <v>  ErrorUnclosedLocationLiteral,    // Error ``    </v>
+        <v>ErrorUnclosedCodeLiteral,    // Error ``</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E75" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B75,",    // ",C75," `",A75,"`    ",D75)</f>
-        <v>  ErrorUnclosedRegularExpression,    // Error ``    </v>
+        <v>ErrorUnclosedLocationLiteral,    // Error ``</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E76" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B76,",    // ",C76," `",A76,"`    ",D76)</f>
-        <v>  ErrorUnclosedTemplate,    // Error ``    </v>
+        <v>ErrorUnclosedRegularExpression,    // Error ``</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E77" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B77,",    // ",C77," `",A77,"`    ",D77)</f>
-        <v>  ErrorUnclosedTextLiteral,    // Error ``    </v>
+        <v>ErrorUnclosedTemplate,    // Error ``</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E78" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B78,",    // ",C78," `",A78,"`    ",D78)</f>
-        <v>  ErrorUnclosedTextLiteralMultiline,    // Error ``    </v>
+        <v>ErrorUnclosedTextLiteral,    // Error ``</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E79" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B79,",    // ",C79," `",A79,"`    ",D79)</f>
-        <v>  ErrorUnexpectedCharacter,    // Error ``    </v>
+        <v>ErrorUnclosedTextLiteralMultiline,    // Error ``</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B80" s="2" t="s">
+      <c r="B80" s="0" t="s">
         <v>115</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>7</v>
+        <v>104</v>
       </c>
       <c r="E80" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B80,",    // ",C80," `",A80,"`    ",D80)</f>
-        <v>  FALSE,    // Keyword `false`    </v>
+        <v>ErrorUnexpectedCharacter,    // Error ``</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="str">
+      <c r="A81" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C81" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E81" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B81,",    // ",C81," `",A81,"`    ",D81)</f>
+        <v>FALSE,    // Keyword `false`</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="str">
         <f aca="false">"%%]"</f>
         <v>%%]</v>
       </c>
-      <c r="B81" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="C81" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="D81" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="E81" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B81,",    // ",C81," `",A81,"`    ",D81)</f>
-        <v>  GRAPH_END,    // Punctuation `%%]`    End of a graph literal</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="str">
+      <c r="B82" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="C82" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D82" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="E82" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B82,",    // ",C82," `",A82,"`    ",D82)</f>
+        <v>GRAPH_END,    // Punctuation `%%]`    End of a graph literal</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="str">
         <f aca="false">"[%%"</f>
         <v>[%%</v>
       </c>
-      <c r="B82" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="C82" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="D82" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="E82" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B82,",    // ",C82," `",A82,"`    ",D82)</f>
-        <v>  GRAPH_START,    // Punctuation `[%%`    Start of a graph literal</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="str">
+      <c r="B83" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="C83" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D83" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="E83" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B83,",    // ",C83," `",A83,"`    ",D83)</f>
+        <v>GRAPH_START,    // Punctuation `[%%`    Start of a graph literal</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="str">
         <f aca="false">"&gt;"</f>
         <v>&gt;</v>
       </c>
-      <c r="B83" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="C83" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="E83" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B83,",    // ",C83," `",A83,"`    ",D83)</f>
-        <v>  GREATER_THAN,    // Operator `&gt;`    </v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="str">
+      <c r="B84" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="C84" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E84" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B84,",    // ",C84," `",A84,"`    ",D84)</f>
+        <v>GREATER_THAN,    // Operator `&gt;`</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="str">
         <f aca="false">"&gt;="</f>
         <v>&gt;=</v>
       </c>
-      <c r="B84" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="C84" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="E84" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B84,",    // ",C84," `",A84,"`    ",D84)</f>
-        <v>  GREATER_THAN_OR_EQUAL,    // Operator `&gt;=`    </v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="B85" s="3" t="s">
+      <c r="B85" s="0" t="s">
         <v>123</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>123</v>
+        <v>51</v>
       </c>
       <c r="E85" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B85,",    // ",C85," `",A85,"`    ",D85)</f>
-        <v>  Identifier,    // Identifier `z_z1`    </v>
+        <v>GREATER_THAN_OR_EQUAL,    // Operator `&gt;=`</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="B86" s="0" t="s">
+      <c r="B86" s="3" t="s">
         <v>125</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>7</v>
+        <v>125</v>
       </c>
       <c r="E86" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B86,",    // ",C86," `",A86,"`    ",D86)</f>
-        <v>  IN,    // Keyword `in`    </v>
+        <v>Identifier,    // Identifier `z_z1`</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="0" t="str">
+      <c r="A87" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="B87" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="C87" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E87" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B87,",    // ",C87," `",A87,"`    ",D87)</f>
+        <v>IN,    // Keyword `in`</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="str">
         <f aca="false">"0b101010"</f>
         <v>0b101010</v>
       </c>
-      <c r="B87" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="C87" s="0" t="s">
+      <c r="B88" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="C88" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="E87" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B87,",    // ",C87," `",A87,"`    ",D87)</f>
-        <v>  IntegerLiteral_Binary,    // Literal `0b101010`    </v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="0" t="str">
+      <c r="E88" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B88,",    // ",C88," `",A88,"`    ",D88)</f>
+        <v>IntegerLiteral_Binary,    // Literal `0b101010`</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="str">
         <f aca="false">"0"</f>
         <v>0</v>
       </c>
-      <c r="B88" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="C88" s="0" t="s">
+      <c r="B89" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="C89" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="E88" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B88,",    // ",C88," `",A88,"`    ",D88)</f>
-        <v>  IntegerLiteral_Decimal,    // Literal `0`    </v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="0" t="str">
+      <c r="E89" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B89,",    // ",C89," `",A89,"`    ",D89)</f>
+        <v>IntegerLiteral_Decimal,    // Literal `0`</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="str">
         <f aca="false">"0x12AB"</f>
         <v>0x12AB</v>
       </c>
-      <c r="B89" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="C89" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E89" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B89,",    // ",C89," `",A89,"`    ",D89)</f>
-        <v>  IntegerLiteral_Hex,    // Literal `0x12AB`    </v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="0" t="s">
-        <v>129</v>
-      </c>
       <c r="B90" s="0" t="s">
         <v>130</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E90" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B90,",    // ",C90," `",A90,"`    ",D90)</f>
-        <v>  IS,    // Keyword `is`    </v>
+        <v>IntegerLiteral_Hex,    // Literal `0x12AB`</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2186,152 +2192,152 @@
       </c>
       <c r="E91" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B91,",    // ",C91," `",A91,"`    ",D91)</f>
-        <v>  ISNOT,    // Keyword `isnot`    </v>
+        <v>IS,    // Keyword `is`</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="0" t="str">
+      <c r="A92" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B92" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="C92" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E92" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B92,",    // ",C92," `",A92,"`    ",D92)</f>
+        <v>ISNOT,    // Keyword `isnot`</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="str">
         <f aca="false">"{"</f>
         <v>{</v>
       </c>
-      <c r="B92" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="C92" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="E92" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B92,",    // ",C92," `",A92,"`    ",D92)</f>
-        <v>  LEFT_BRACE,    // Punctuation `{`    </v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="0" t="str">
+      <c r="B93" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="C93" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="E93" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B93,",    // ",C93," `",A93,"`    ",D93)</f>
+        <v>LEFT_BRACE,    // Punctuation `{`</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="str">
         <f aca="false">"["</f>
         <v>[</v>
       </c>
-      <c r="B93" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="C93" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="E93" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B93,",    // ",C93," `",A93,"`    ",D93)</f>
-        <v>  LEFT_BRACKET,    // Punctuation `[`    </v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="0" t="str">
+      <c r="B94" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="C94" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="E94" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B94,",    // ",C94," `",A94,"`    ",D94)</f>
+        <v>LEFT_BRACKET,    // Punctuation `[`</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="str">
         <f aca="false">"("</f>
         <v>(</v>
       </c>
-      <c r="B94" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="C94" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="E94" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B94,",    // ",C94," `",A94,"`    ",D94)</f>
-        <v>  LEFT_PARENTHESIS,    // Punctuation `(`    </v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="0" t="str">
+      <c r="B95" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="C95" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="E95" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B95,",    // ",C95," `",A95,"`    ",D95)</f>
+        <v>LEFT_PARENTHESIS,    // Punctuation `(`</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="str">
         <f aca="false">"&lt;"</f>
         <v>&lt;</v>
       </c>
-      <c r="B95" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="C95" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="E95" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B95,",    // ",C95," `",A95,"`    ",D95)</f>
-        <v>  LESS_THAN,    // Operator `&lt;`    </v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="0" t="str">
+      <c r="B96" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="C96" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E96" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B96,",    // ",C96," `",A96,"`    ",D96)</f>
+        <v>LESS_THAN,    // Operator `&lt;`</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="str">
         <f aca="false">"&lt;="</f>
         <v>&lt;=</v>
       </c>
-      <c r="B96" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="C96" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="E96" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B96,",    // ",C96," `",A96,"`    ",D96)</f>
-        <v>  LESS_THAN_OR_EQUAL,    // Operator `&lt;=`    </v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="0" t="str">
+      <c r="B97" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="C97" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E97" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B97,",    // ",C97," `",A97,"`    ",D97)</f>
+        <v>LESS_THAN_OR_EQUAL,    // Operator `&lt;=`</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="str">
         <f aca="false">"@| ... |"</f>
         <v>@| ... |</v>
       </c>
-      <c r="B97" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="C97" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E97" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B97,",    // ",C97," `",A97,"`    ",D97)</f>
-        <v>  LocationLiteral,    // Literal `@| ... |`    </v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="0" t="s">
-        <v>139</v>
-      </c>
       <c r="B98" s="0" t="s">
         <v>140</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D98" s="0" t="s">
-        <v>141</v>
+        <v>9</v>
       </c>
       <c r="E98" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B98,",    // ",C98," `",A98,"`    ",D98)</f>
-        <v>  MINUS,    // Operator `-`    Subtraction (infix); Negation (prefix)</v>
+        <v>LocationLiteral,    // Literal `@| ... |`</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="0" t="str">
+      <c r="A99" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B99" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="C99" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D99" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E99" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B99,",    // ",C99," `",A99,"`    ",D99)</f>
+        <v>MINUS,    // Operator `-`    Subtraction (infix); Negation (prefix)</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="str">
         <f aca="false">"-="</f>
         <v>-=</v>
       </c>
-      <c r="B99" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="C99" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="E99" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B99,",    // ",C99," `",A99,"`    ",D99)</f>
-        <v>  MINUS_EQUALS,    // Operator `-=`    </v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="0" t="s">
-        <v>143</v>
-      </c>
       <c r="B100" s="0" t="s">
         <v>144</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="E100" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B100,",    // ",C100," `",A100,"`    ",D100)</f>
-        <v>  MOD,    // Keyword `mod`    </v>
+        <v>MINUS_EQUALS,    // Operator `-=`</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2346,515 +2352,515 @@
       </c>
       <c r="E101" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B101,",    // ",C101," `",A101,"`    ",D101)</f>
-        <v>  NOT,    // Keyword `not`    </v>
+        <v>MOD,    // Keyword `mod`</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="0" t="str">
+      <c r="A102" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="B102" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="C102" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E102" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B102,",    // ",C102," `",A102,"`    ",D102)</f>
+        <v>NOT,    // Keyword `not`</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="str">
         <f aca="false">"&lt;&gt;"</f>
         <v>&lt;&gt;</v>
       </c>
-      <c r="B102" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="C102" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="E102" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B102,",    // ",C102," `",A102,"`    ",D102)</f>
-        <v>  NOT_EQUAL_TO,    // Operator `&lt;&gt;`    </v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="0" t="s">
-        <v>148</v>
-      </c>
       <c r="B103" s="0" t="s">
         <v>149</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="E103" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B103,",    // ",C103," `",A103,"`    ",D103)</f>
-        <v>  NOTIN,    // Keyword `notin`    </v>
+        <v>NOT_EQUAL_TO,    // Operator `&lt;&gt;`</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="0" t="str">
+      <c r="A104" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B104" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="C104" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E104" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B104,",    // ",C104," `",A104,"`    ",D104)</f>
+        <v>NOTIN,    // Keyword `notin`</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="str">
         <f aca="false">"123.45"</f>
         <v>123.45</v>
       </c>
-      <c r="B104" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="C104" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E104" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B104,",    // ",C104," `",A104,"`    ",D104)</f>
-        <v>  NumberLiteral,    // Literal `123.45`    </v>
-      </c>
-    </row>
-    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="0" t="s">
-        <v>151</v>
-      </c>
       <c r="B105" s="0" t="s">
         <v>152</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E105" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B105,",    // ",C105," `",A105,"`    ",D105)</f>
-        <v>  OR,    // Keyword `or`    </v>
+        <v>NumberLiteral,    // Literal `123.45`</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="0" t="str">
+      <c r="A106" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B106" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="C106" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E106" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B106,",    // ",C106," `",A106,"`    ",D106)</f>
+        <v>OR,    // Keyword `or`</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="str">
         <f aca="false">"%"</f>
         <v>%</v>
       </c>
-      <c r="B106" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="C106" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="E106" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B106,",    // ",C106," `",A106,"`    ",D106)</f>
-        <v>  PERCENT,    // Operator `%`    </v>
-      </c>
-    </row>
-    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="0" t="str">
+      <c r="B107" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="C107" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E107" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B107,",    // ",C107," `",A107,"`    ",D107)</f>
+        <v>PERCENT,    // Operator `%`</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="str">
         <f aca="false">"+"</f>
         <v>+</v>
       </c>
-      <c r="B107" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="C107" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="E107" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B107,",    // ",C107," `",A107,"`    ",D107)</f>
-        <v>  PLUS,    // Operator `+`    </v>
-      </c>
-    </row>
-    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="0" t="str">
+      <c r="B108" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="C108" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E108" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B108,",    // ",C108," `",A108,"`    ",D108)</f>
+        <v>PLUS,    // Operator `+`</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="str">
         <f aca="false">"+="</f>
         <v>+=</v>
       </c>
-      <c r="B108" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="C108" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="E108" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B108,",    // ",C108," `",A108,"`    ",D108)</f>
-        <v>  PLUS_EQUALS,    // Operator `+=`    </v>
-      </c>
-    </row>
-    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="0" t="str">
+      <c r="B109" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="C109" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E109" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B109,",    // ",C109," `",A109,"`    ",D109)</f>
+        <v>PLUS_EQUALS,    // Operator `+=`</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="str">
         <f aca="false">"^"</f>
         <v>^</v>
       </c>
-      <c r="B109" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="C109" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="E109" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B109,",    // ",C109," `",A109,"`    ",D109)</f>
-        <v>  POWER,    // Operator `^`    </v>
-      </c>
-    </row>
-    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="0" t="str">
+      <c r="B110" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="C110" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E110" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B110,",    // ",C110," `",A110,"`    ",D110)</f>
+        <v>POWER,    // Operator `^`</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="0" t="str">
         <f aca="false">"^="</f>
         <v>^=</v>
       </c>
-      <c r="B110" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="C110" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="E110" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B110,",    // ",C110," `",A110,"`    ",D110)</f>
-        <v>  POWER_EQUALS,    // Operator `^=`    </v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="0" t="str">
+      <c r="B111" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="C111" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E111" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B111,",    // ",C111," `",A111,"`    ",D111)</f>
+        <v>POWER_EQUALS,    // Operator `^=`</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="str">
         <f aca="false">"?"</f>
         <v>?</v>
       </c>
-      <c r="B111" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="C111" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="E111" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B111,",    // ",C111," `",A111,"`    ",D111)</f>
-        <v>  QUESTION,    // Punctuation `?`    </v>
-      </c>
-    </row>
-    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="0" t="s">
-        <v>159</v>
-      </c>
       <c r="B112" s="0" t="s">
         <v>160</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D112" s="0" t="s">
-        <v>161</v>
+        <v>83</v>
       </c>
       <c r="E112" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B112,",    // ",C112," `",A112,"`    ",D112)</f>
-        <v>  QUESTION_QUESTION,    // Operator `??`    Null coalescence</v>
+        <v>QUESTION,    // Punctuation `?`</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="0" t="str">
+      <c r="A113" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="B113" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="C113" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D113" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="E113" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B113,",    // ",C113," `",A113,"`    ",D113)</f>
+        <v>QUESTION_QUESTION,    // Operator `??`    Null coalescence</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="str">
         <f aca="false">"..&lt;"</f>
         <v>..&lt;</v>
       </c>
-      <c r="B113" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="C113" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D113" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="E113" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B113,",    // ",C113," `",A113,"`    ",D113)</f>
-        <v>  RANGE_EXCLUSIVE,    // Operator `..&lt;`    Range from lower inclusive to upper exclusive</v>
-      </c>
-    </row>
-    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="0" t="str">
+      <c r="B114" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="C114" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D114" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="E114" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B114,",    // ",C114," `",A114,"`    ",D114)</f>
+        <v>RANGE_EXCLUSIVE,    // Operator `..&lt;`    Range from lower inclusive to upper exclusive</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="str">
         <f aca="false">".."</f>
         <v>..</v>
       </c>
-      <c r="B114" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="C114" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D114" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="E114" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B114,",    // ",C114," `",A114,"`    ",D114)</f>
-        <v>  RANGE_INCLUSIVE,    // Operator `..`    Range from lower to upper inclusive</v>
-      </c>
-    </row>
-    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="0" t="str">
+      <c r="B115" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="C115" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D115" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="E115" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B115,",    // ",C115," `",A115,"`    ",D115)</f>
+        <v>RANGE_INCLUSIVE,    // Operator `..`    Range from lower to upper inclusive</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="str">
         <f aca="false">"~/ ... /igm"</f>
         <v>~/ ... /igm</v>
       </c>
-      <c r="B115" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="C115" s="0" t="s">
+      <c r="B116" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="C116" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="E115" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B115,",    // ",C115," `",A115,"`    ",D115)</f>
-        <v>  RegularExpressionLiteral,    // Literal `~/ ... /igm`    </v>
-      </c>
-    </row>
-    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="0" t="str">
+      <c r="E116" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B116,",    // ",C116," `",A116,"`    ",D116)</f>
+        <v>RegularExpressionLiteral,    // Literal `~/ ... /igm`</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="str">
         <f aca="false">"}"</f>
         <v>}</v>
       </c>
-      <c r="B116" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="C116" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="E116" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B116,",    // ",C116," `",A116,"`    ",D116)</f>
-        <v>  RIGHT_BRACE,    // Punctuation `}`    </v>
-      </c>
-    </row>
-    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="0" t="str">
+      <c r="B117" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="C117" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="E117" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B117,",    // ",C117," `",A117,"`    ",D117)</f>
+        <v>RIGHT_BRACE,    // Punctuation `}`</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="str">
         <f aca="false">"]"</f>
         <v>]</v>
       </c>
-      <c r="B117" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="C117" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="E117" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B117,",    // ",C117," `",A117,"`    ",D117)</f>
-        <v>  RIGHT_BRACKET,    // Punctuation `]`    </v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="0" t="str">
+      <c r="B118" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="C118" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="E118" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B118,",    // ",C118," `",A118,"`    ",D118)</f>
+        <v>RIGHT_BRACKET,    // Punctuation `]`</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="str">
         <f aca="false">")"</f>
         <v>)</v>
       </c>
-      <c r="B118" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="C118" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="E118" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B118,",    // ",C118," `",A118,"`    ",D118)</f>
-        <v>  RIGHT_PARENTHESIS,    // Punctuation `)`    </v>
-      </c>
-    </row>
-    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="0" t="s">
-        <v>170</v>
-      </c>
       <c r="B119" s="0" t="s">
         <v>171</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>7</v>
+        <v>83</v>
       </c>
       <c r="E119" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B119,",    // ",C119," `",A119,"`    ",D119)</f>
-        <v>  SELF,    // Keyword `self`    </v>
+        <v>RIGHT_PARENTHESIS,    // Punctuation `)`</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="0" t="str">
+      <c r="A120" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="B120" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="C120" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E120" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B120,",    // ",C120," `",A120,"`    ",D120)</f>
+        <v>SELF,    // Keyword `self`</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="str">
         <f aca="false">";"</f>
         <v>;</v>
       </c>
-      <c r="B120" s="0" t="s">
-        <v>172</v>
-      </c>
-      <c r="C120" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="E120" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B120,",    // ",C120," `",A120,"`    ",D120)</f>
-        <v>  SEMICOLON,    // Punctuation `;`    </v>
-      </c>
-    </row>
-    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="0" t="s">
-        <v>173</v>
-      </c>
       <c r="B121" s="0" t="s">
         <v>174</v>
       </c>
       <c r="C121" s="0" t="s">
-        <v>174</v>
+        <v>83</v>
       </c>
       <c r="E121" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B121,",    // ",C121," `",A121,"`    ",D121)</f>
-        <v>  Tag,    // Tag `#abc_def`    </v>
+        <v>SEMICOLON,    // Punctuation `;`</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="0" t="str">
+      <c r="A122" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="B122" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="C122" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="E122" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B122,",    // ",C122," `",A122,"`    ",D122)</f>
+        <v>Tag,    // Tag `#abc_def`</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="str">
         <f aca="false">"{{{...}}}"</f>
         <v>{{{...}}}</v>
       </c>
-      <c r="B122" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="C122" s="0" t="s">
+      <c r="B123" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C123" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="E122" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B122,",    // ",C122," `",A122,"`    ",D122)</f>
-        <v>  TemplateLiteral,    // Literal `{{{...}}}`    </v>
-      </c>
-    </row>
-    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="0" t="str">
+      <c r="E123" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B123,",    // ",C123," `",A123,"`    ",D123)</f>
+        <v>TemplateLiteral,    // Literal `{{{...}}}`</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="0" t="str">
         <f aca="false">"""..."""</f>
         <v>"..."</v>
       </c>
-      <c r="B123" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="C123" s="0" t="s">
+      <c r="B124" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="C124" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="E123" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B123,",    // ",C123," `",A123,"`    ",D123)</f>
-        <v>  TextLiteral_DoubleQuoted,    // Literal `"..."`    </v>
-      </c>
-    </row>
-    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="0" t="str">
+      <c r="E124" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B124,",    // ",C124," `",A124,"`    ",D124)</f>
+        <v>TextLiteral_DoubleQuoted,    // Literal `"..."`</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="0" t="str">
         <f aca="false">"""""""..."""""""</f>
         <v>"""..."""</v>
       </c>
-      <c r="B124" s="0" t="s">
-        <v>177</v>
-      </c>
-      <c r="C124" s="0" t="s">
+      <c r="B125" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="C125" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="E124" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B124,",    // ",C124," `",A124,"`    ",D124)</f>
-        <v>  TextLiteral_DoubleQuotedMultiline,    // Literal `"""..."""`    </v>
-      </c>
-    </row>
-    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="0" t="str">
+      <c r="E125" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B125,",    // ",C125," `",A125,"`    ",D125)</f>
+        <v>TextLiteral_DoubleQuotedMultiline,    // Literal `"""..."""`</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="0" t="str">
         <f aca="false">"'...'"</f>
         <v>'...'</v>
       </c>
-      <c r="B125" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="C125" s="0" t="s">
+      <c r="B126" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="C126" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="E125" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B125,",    // ",C125," `",A125,"`    ",D125)</f>
-        <v>  TextLiteral_SingleQuoted,    // Literal `'...'`    </v>
-      </c>
-    </row>
-    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="0" t="str">
+      <c r="E126" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B126,",    // ",C126," `",A126,"`    ",D126)</f>
+        <v>TextLiteral_SingleQuoted,    // Literal `'...'`</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="0" t="str">
         <f aca="false">"'''...'''"</f>
         <v>'''...'''</v>
       </c>
-      <c r="B126" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="C126" s="0" t="s">
+      <c r="B127" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="C127" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="E126" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B126,",    // ",C126," `",A126,"`    ",D126)</f>
-        <v>  TextLiteral_SingleQuotedMultiline,    // Literal `'''...'''`    </v>
-      </c>
-    </row>
-    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="0" t="str">
+      <c r="E127" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B127,",    // ",C127," `",A127,"`    ",D127)</f>
+        <v>TextLiteral_SingleQuotedMultiline,    // Literal `'''...'''`</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="0" t="str">
         <f aca="false">"~"</f>
         <v>~</v>
       </c>
-      <c r="B127" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="C127" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="E127" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B127,",    // ",C127," `",A127,"`    ",D127)</f>
-        <v>  TILDE,    // Operator `~`    </v>
-      </c>
-    </row>
-    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="0" t="str">
+      <c r="B128" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="C128" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E128" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B128,",    // ",C128," `",A128,"`    ",D128)</f>
+        <v>TILDE,    // Operator `~`</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="0" t="str">
         <f aca="false">"~="</f>
         <v>~=</v>
       </c>
-      <c r="B128" s="0" t="s">
-        <v>181</v>
-      </c>
-      <c r="C128" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="E128" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B128,",    // ",C128," `",A128,"`    ",D128)</f>
-        <v>  TILDE_EQUALS,    // Operator `~=`    </v>
-      </c>
-    </row>
-    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="0" t="str">
+      <c r="B129" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="C129" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E129" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B129,",    // ",C129," `",A129,"`    ",D129)</f>
+        <v>TILDE_EQUALS,    // Operator `~=`</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="0" t="str">
         <f aca="false">"*"</f>
         <v>*</v>
       </c>
-      <c r="B129" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="C129" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="E129" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B129,",    // ",C129," `",A129,"`    ",D129)</f>
-        <v>  TIMES,    // Operator `*`    </v>
-      </c>
-    </row>
-    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="0" t="str">
+      <c r="B130" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="C130" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E130" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B130,",    // ",C130," `",A130,"`    ",D130)</f>
+        <v>TIMES,    // Operator `*`</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="0" t="str">
         <f aca="false">"*="</f>
         <v>*=</v>
       </c>
-      <c r="B130" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="C130" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="E130" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B130,",    // ",C130," `",A130,"`    ",D130)</f>
-        <v>  TIMES_EQUALS,    // Operator `*=`    </v>
-      </c>
-    </row>
-    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="0" t="s">
-        <v>184</v>
-      </c>
       <c r="B131" s="0" t="s">
         <v>185</v>
       </c>
       <c r="C131" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="D131" s="0" t="s">
-        <v>186</v>
-      </c>
       <c r="E131" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B131,",    // ",C131," `",A131,"`    ",D131)</f>
-        <v>  TO_STRING,    // Operator `$`    Conversion to string (prefix)</v>
+        <v>TIMES_EQUALS,    // Operator `*=`</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="2" t="s">
+      <c r="A132" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="B132" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="B132" s="2" t="s">
+      <c r="C132" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D132" s="0" t="s">
         <v>188</v>
-      </c>
-      <c r="C132" s="0" t="s">
-        <v>7</v>
       </c>
       <c r="E132" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B132,",    // ",C132," `",A132,"`    ",D132)</f>
-        <v>  TRUE,    // Keyword `true`    </v>
+        <v>TO_STRING,    // Operator `$`    Conversion to string (prefix)</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="0" t="s">
+      <c r="A133" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B133" s="0" t="s">
+      <c r="B133" s="2" t="s">
         <v>190</v>
       </c>
       <c r="C133" s="0" t="s">
@@ -2862,7 +2868,7 @@
       </c>
       <c r="E133" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B133,",    // ",C133," `",A133,"`    ",D133)</f>
-        <v>  UNDEFINED,    // Keyword `undefined`    </v>
+        <v>TRUE,    // Keyword `true`</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2877,95 +2883,110 @@
       </c>
       <c r="E134" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B134,",    // ",C134," `",A134,"`    ",D134)</f>
-        <v>  USE,    // Keyword `use`    </v>
+        <v>UNDEFINED,    // Keyword `undefined`</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="0" t="str">
+      <c r="A135" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="B135" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="C135" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E135" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B135,",    // ",C135," `",A135,"`    ",D135)</f>
+        <v>USE,    // Keyword `use`</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="0" t="str">
         <f aca="false">"#{...}"</f>
         <v>#{...}</v>
       </c>
-      <c r="B135" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="C135" s="0" t="s">
+      <c r="B136" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="C136" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="D135" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="E135" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B135,",    // ",C135," `",A135,"`    ",D135)</f>
-        <v>  UserDefinedLiteral_Braces,    // Literal `#{...}`    User-defined literal B</v>
-      </c>
-    </row>
-    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="0" t="str">
+      <c r="D136" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="E136" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B136,",    // ",C136," `",A136,"`    ",D136)</f>
+        <v>UserDefinedLiteral_Braces,    // Literal `#{...}`    User-defined literal B</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="0" t="str">
         <f aca="false">"#[...]"</f>
         <v>#[...]</v>
       </c>
-      <c r="B136" s="0" t="s">
-        <v>195</v>
-      </c>
-      <c r="C136" s="0" t="s">
+      <c r="B137" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="C137" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="D136" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="E136" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B136,",    // ",C136," `",A136,"`    ",D136)</f>
-        <v>  UserDefinedLiteral_Brackets,    // Literal `#[...]`    User-defined literal A</v>
-      </c>
-    </row>
-    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="0" t="str">
+      <c r="D137" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="E137" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B137,",    // ",C137," `",A137,"`    ",D137)</f>
+        <v>UserDefinedLiteral_Brackets,    // Literal `#[...]`    User-defined literal A</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="0" t="str">
         <f aca="false">"#/.../"</f>
         <v>#/.../</v>
       </c>
-      <c r="B137" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="C137" s="0" t="s">
+      <c r="B138" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="C138" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="D137" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="E137" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B137,",    // ",C137," `",A137,"`    ",D137)</f>
-        <v>  UserDefinedLiteral_Slashes,    // Literal `#/.../`    User-defined literal C</v>
-      </c>
-    </row>
-    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="0" t="str">
+      <c r="D138" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="E138" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B138,",    // ",C138," `",A138,"`    ",D138)</f>
+        <v>UserDefinedLiteral_Slashes,    // Literal `#/.../`    User-defined literal C</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="0" t="str">
         <f aca="false">"2.3.4"</f>
         <v>2.3.4</v>
       </c>
-      <c r="B138" s="0" t="s">
-        <v>199</v>
-      </c>
-      <c r="C138" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E138" s="0" t="str">
-        <f aca="false">CONCATENATE("  ",B138,",    // ",C138," `",A138,"`    ",D138)</f>
-        <v>  VersionLiteral,    // Literal `2.3.4`    </v>
-      </c>
-    </row>
-    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="0" t="s">
-        <v>200</v>
-      </c>
       <c r="B139" s="0" t="s">
         <v>201</v>
       </c>
       <c r="C139" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E139" s="0" t="str">
         <f aca="false">CONCATENATE("  ",B139,",    // ",C139," `",A139,"`    ",D139)</f>
-        <v>  XOR,    // Keyword `xor`    </v>
+        <v>VersionLiteral,    // Literal `2.3.4`</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="B140" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="C140" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E140" s="0" t="str">
+        <f aca="false">CONCATENATE("  ",B140,",    // ",C140," `",A140,"`    ",D140)</f>
+        <v>XOR,    // Keyword `xor`</v>
       </c>
     </row>
   </sheetData>

</xml_diff>